<commit_message>
enny06 2019/09/02 09.35 Update print excel master item
</commit_message>
<xml_diff>
--- a/assets/templates/template_items_log.xlsx
+++ b/assets/templates/template_items_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\greebel\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB2D20A-3B4F-4341-AF2D-BA11E4B15E27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0B2D63-2284-4371-99C3-C53DD239001F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2D745729-4032-447E-85FB-C820FC51974E}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:O110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:L6"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +552,7 @@
       <c r="I4" s="12"/>
       <c r="J4" s="14">
         <f ca="1">NOW()</f>
-        <v>43707.76719259259</v>
+        <v>43710.360099421297</v>
       </c>
       <c r="K4" s="14"/>
       <c r="L4" s="14"/>
@@ -597,8 +597,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
+      <c r="M7" s="2"/>
       <c r="O7" s="3"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -614,6 +613,7 @@
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
@@ -628,6 +628,7 @@
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
@@ -642,6 +643,7 @@
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
@@ -656,6 +658,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
@@ -670,6 +673,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
@@ -684,6 +688,7 @@
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
@@ -698,6 +703,7 @@
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
@@ -712,6 +718,7 @@
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
@@ -726,8 +733,9 @@
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -740,8 +748,9 @@
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
@@ -754,8 +763,9 @@
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
@@ -768,8 +778,9 @@
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
@@ -782,8 +793,9 @@
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="8"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
@@ -796,8 +808,9 @@
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
@@ -810,8 +823,9 @@
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="8"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
@@ -824,8 +838,9 @@
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="8"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
@@ -838,8 +853,9 @@
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="8"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
@@ -852,8 +868,9 @@
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="8"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
@@ -866,8 +883,9 @@
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" s="8"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
@@ -880,8 +898,9 @@
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" s="8"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
@@ -894,8 +913,9 @@
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" s="8"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
@@ -908,8 +928,9 @@
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" s="8"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
@@ -922,8 +943,9 @@
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30" s="8"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
@@ -936,8 +958,9 @@
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31" s="8"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
@@ -950,8 +973,9 @@
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32" s="8"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
@@ -964,8 +988,9 @@
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33" s="8"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
@@ -978,8 +1003,9 @@
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34" s="8"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
@@ -992,8 +1018,9 @@
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35" s="8"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
@@ -1006,8 +1033,9 @@
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36" s="8"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
@@ -1020,8 +1048,9 @@
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37" s="8"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="7"/>
@@ -1034,8 +1063,9 @@
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M38" s="8"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>
@@ -1048,8 +1078,9 @@
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M39" s="8"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="7"/>
@@ -1062,8 +1093,9 @@
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40" s="8"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="7"/>
@@ -1076,8 +1108,9 @@
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M41" s="8"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="7"/>
@@ -1090,8 +1123,9 @@
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42" s="8"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="7"/>
@@ -1104,8 +1138,9 @@
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M43" s="8"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
@@ -1118,8 +1153,9 @@
       <c r="J44" s="8"/>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M44" s="8"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="7"/>
@@ -1132,8 +1168,9 @@
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M45" s="8"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="E46" s="4"/>
@@ -1142,8 +1179,9 @@
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M46" s="8"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="E47" s="4"/>
@@ -1152,8 +1190,9 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M47" s="8"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="E48" s="4"/>
@@ -1162,8 +1201,9 @@
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M48" s="8"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="E49" s="4"/>
@@ -1172,8 +1212,9 @@
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M49" s="8"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="E50" s="4"/>
@@ -1182,8 +1223,9 @@
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M50" s="8"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="E51" s="4"/>
@@ -1192,8 +1234,9 @@
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M51" s="8"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="E52" s="4"/>
@@ -1202,8 +1245,9 @@
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M52" s="8"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="E53" s="4"/>
@@ -1212,8 +1256,9 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M53" s="8"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="E54" s="4"/>
@@ -1222,8 +1267,9 @@
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M54" s="8"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="E55" s="4"/>
@@ -1232,8 +1278,9 @@
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M55" s="8"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="E56" s="4"/>
@@ -1242,8 +1289,9 @@
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M56" s="8"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
       <c r="E57" s="4"/>
@@ -1252,8 +1300,9 @@
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M57" s="8"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="E58" s="4"/>
@@ -1262,8 +1311,9 @@
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M58" s="8"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="E59" s="4"/>
@@ -1272,8 +1322,9 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M59" s="8"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="E60" s="4"/>
@@ -1282,8 +1333,9 @@
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M60" s="8"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="E61" s="4"/>
@@ -1292,8 +1344,9 @@
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M61" s="8"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="E62" s="4"/>
@@ -1302,8 +1355,9 @@
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M62" s="8"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
       <c r="E63" s="4"/>
@@ -1312,8 +1366,9 @@
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M63" s="8"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
       <c r="E64" s="4"/>
@@ -1322,8 +1377,9 @@
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M64" s="8"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="E65" s="4"/>
       <c r="G65" s="4"/>
@@ -1331,8 +1387,9 @@
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
       <c r="L65" s="4"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M65" s="8"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="E66" s="4"/>
       <c r="G66" s="4"/>
@@ -1340,8 +1397,9 @@
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M66" s="8"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="E67" s="4"/>
       <c r="G67" s="4"/>
@@ -1349,8 +1407,9 @@
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M67" s="8"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="E68" s="4"/>
       <c r="G68" s="4"/>
@@ -1358,8 +1417,9 @@
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
       <c r="L68" s="4"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M68" s="8"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="E69" s="4"/>
       <c r="G69" s="4"/>
@@ -1367,8 +1427,9 @@
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M69" s="8"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="E70" s="4"/>
       <c r="G70" s="4"/>
@@ -1376,8 +1437,9 @@
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M70" s="8"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="E71" s="4"/>
       <c r="G71" s="4"/>
@@ -1385,8 +1447,9 @@
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
       <c r="L71" s="4"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M71" s="8"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="E72" s="4"/>
       <c r="G72" s="4"/>
@@ -1394,8 +1457,9 @@
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
       <c r="L72" s="4"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M72" s="8"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="E73" s="4"/>
       <c r="G73" s="4"/>
@@ -1403,8 +1467,9 @@
       <c r="J73" s="4"/>
       <c r="K73" s="4"/>
       <c r="L73" s="4"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M73" s="8"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="E74" s="4"/>
       <c r="G74" s="4"/>
@@ -1412,8 +1477,9 @@
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
       <c r="L74" s="4"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M74" s="8"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="E75" s="4"/>
       <c r="G75" s="4"/>
@@ -1421,8 +1487,9 @@
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
       <c r="L75" s="4"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M75" s="8"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="E76" s="4"/>
       <c r="G76" s="4"/>
@@ -1430,8 +1497,9 @@
       <c r="J76" s="4"/>
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M76" s="8"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="E77" s="4"/>
       <c r="G77" s="4"/>
@@ -1439,8 +1507,9 @@
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
       <c r="L77" s="4"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M77" s="8"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="E78" s="4"/>
       <c r="G78" s="4"/>
@@ -1448,8 +1517,9 @@
       <c r="J78" s="4"/>
       <c r="K78" s="4"/>
       <c r="L78" s="4"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M78" s="8"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="E79" s="4"/>
       <c r="G79" s="4"/>
@@ -1457,8 +1527,9 @@
       <c r="J79" s="4"/>
       <c r="K79" s="4"/>
       <c r="L79" s="4"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M79" s="8"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="E80" s="4"/>
       <c r="G80" s="4"/>
@@ -1466,8 +1537,9 @@
       <c r="J80" s="4"/>
       <c r="K80" s="4"/>
       <c r="L80" s="4"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M80" s="8"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="E81" s="4"/>
       <c r="G81" s="4"/>
@@ -1475,8 +1547,9 @@
       <c r="J81" s="4"/>
       <c r="K81" s="4"/>
       <c r="L81" s="4"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M81" s="8"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="E82" s="4"/>
       <c r="G82" s="4"/>
@@ -1484,8 +1557,9 @@
       <c r="J82" s="4"/>
       <c r="K82" s="4"/>
       <c r="L82" s="4"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M82" s="8"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="E83" s="4"/>
       <c r="G83" s="4"/>
@@ -1493,8 +1567,9 @@
       <c r="J83" s="4"/>
       <c r="K83" s="4"/>
       <c r="L83" s="4"/>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M83" s="8"/>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="E84" s="4"/>
       <c r="G84" s="4"/>
@@ -1502,8 +1577,9 @@
       <c r="J84" s="4"/>
       <c r="K84" s="4"/>
       <c r="L84" s="4"/>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M84" s="8"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="E85" s="4"/>
       <c r="G85" s="4"/>
@@ -1511,8 +1587,9 @@
       <c r="J85" s="4"/>
       <c r="K85" s="4"/>
       <c r="L85" s="4"/>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M85" s="8"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="E86" s="4"/>
       <c r="G86" s="4"/>
@@ -1520,8 +1597,9 @@
       <c r="J86" s="4"/>
       <c r="K86" s="4"/>
       <c r="L86" s="4"/>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M86" s="8"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="E87" s="4"/>
       <c r="G87" s="4"/>
@@ -1529,8 +1607,9 @@
       <c r="J87" s="4"/>
       <c r="K87" s="4"/>
       <c r="L87" s="4"/>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M87" s="8"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="E88" s="4"/>
       <c r="G88" s="4"/>
@@ -1538,8 +1617,9 @@
       <c r="J88" s="4"/>
       <c r="K88" s="4"/>
       <c r="L88" s="4"/>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M88" s="8"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="E89" s="4"/>
       <c r="G89" s="4"/>
@@ -1547,8 +1627,9 @@
       <c r="J89" s="4"/>
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M89" s="8"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="E90" s="4"/>
       <c r="G90" s="4"/>
@@ -1556,8 +1637,9 @@
       <c r="J90" s="4"/>
       <c r="K90" s="4"/>
       <c r="L90" s="4"/>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M90" s="8"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="E91" s="4"/>
       <c r="G91" s="4"/>
@@ -1565,8 +1647,9 @@
       <c r="J91" s="4"/>
       <c r="K91" s="4"/>
       <c r="L91" s="4"/>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M91" s="8"/>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
       <c r="E92" s="4"/>
       <c r="G92" s="4"/>
@@ -1574,8 +1657,9 @@
       <c r="J92" s="4"/>
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M92" s="8"/>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="E93" s="4"/>
       <c r="G93" s="4"/>
@@ -1583,8 +1667,9 @@
       <c r="J93" s="4"/>
       <c r="K93" s="4"/>
       <c r="L93" s="4"/>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M93" s="8"/>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
       <c r="E94" s="4"/>
       <c r="G94" s="4"/>
@@ -1592,8 +1677,9 @@
       <c r="J94" s="4"/>
       <c r="K94" s="4"/>
       <c r="L94" s="4"/>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M94" s="8"/>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="E95" s="4"/>
       <c r="G95" s="4"/>
@@ -1601,8 +1687,9 @@
       <c r="J95" s="4"/>
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M95" s="8"/>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
       <c r="E96" s="4"/>
       <c r="G96" s="4"/>
@@ -1610,8 +1697,9 @@
       <c r="J96" s="4"/>
       <c r="K96" s="4"/>
       <c r="L96" s="4"/>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M96" s="8"/>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
       <c r="E97" s="4"/>
       <c r="G97" s="4"/>
@@ -1619,8 +1707,9 @@
       <c r="J97" s="4"/>
       <c r="K97" s="4"/>
       <c r="L97" s="4"/>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M97" s="8"/>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
       <c r="E98" s="4"/>
       <c r="G98" s="4"/>
@@ -1628,8 +1717,9 @@
       <c r="J98" s="4"/>
       <c r="K98" s="4"/>
       <c r="L98" s="4"/>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M98" s="8"/>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="E99" s="4"/>
       <c r="G99" s="4"/>
@@ -1637,8 +1727,9 @@
       <c r="J99" s="4"/>
       <c r="K99" s="4"/>
       <c r="L99" s="4"/>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M99" s="8"/>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="5"/>
       <c r="E100" s="4"/>
       <c r="G100" s="4"/>
@@ -1646,8 +1737,9 @@
       <c r="J100" s="4"/>
       <c r="K100" s="4"/>
       <c r="L100" s="4"/>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M100" s="8"/>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
       <c r="E101" s="4"/>
       <c r="G101" s="4"/>
@@ -1655,8 +1747,9 @@
       <c r="J101" s="4"/>
       <c r="K101" s="4"/>
       <c r="L101" s="4"/>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M101" s="8"/>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
       <c r="E102" s="4"/>
       <c r="G102" s="4"/>
@@ -1664,8 +1757,9 @@
       <c r="J102" s="4"/>
       <c r="K102" s="4"/>
       <c r="L102" s="4"/>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M102" s="8"/>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
       <c r="E103" s="4"/>
       <c r="G103" s="4"/>
@@ -1673,8 +1767,9 @@
       <c r="J103" s="4"/>
       <c r="K103" s="4"/>
       <c r="L103" s="4"/>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M103" s="8"/>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="E104" s="4"/>
       <c r="G104" s="4"/>
@@ -1682,8 +1777,9 @@
       <c r="J104" s="4"/>
       <c r="K104" s="4"/>
       <c r="L104" s="4"/>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M104" s="8"/>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
       <c r="E105" s="4"/>
       <c r="G105" s="4"/>
@@ -1691,8 +1787,9 @@
       <c r="J105" s="4"/>
       <c r="K105" s="4"/>
       <c r="L105" s="4"/>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M105" s="8"/>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
       <c r="E106" s="4"/>
       <c r="G106" s="4"/>
@@ -1700,8 +1797,9 @@
       <c r="J106" s="4"/>
       <c r="K106" s="4"/>
       <c r="L106" s="4"/>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M106" s="8"/>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
       <c r="E107" s="4"/>
       <c r="G107" s="4"/>
@@ -1709,30 +1807,34 @@
       <c r="J107" s="4"/>
       <c r="K107" s="4"/>
       <c r="L107" s="4"/>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M107" s="8"/>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E108" s="4"/>
       <c r="G108" s="4"/>
       <c r="I108" s="4"/>
       <c r="J108" s="4"/>
       <c r="K108" s="4"/>
       <c r="L108" s="4"/>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M108" s="8"/>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E109" s="4"/>
       <c r="G109" s="4"/>
       <c r="I109" s="4"/>
       <c r="J109" s="4"/>
       <c r="K109" s="4"/>
       <c r="L109" s="4"/>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M109" s="8"/>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E110" s="4"/>
       <c r="G110" s="4"/>
       <c r="I110" s="4"/>
       <c r="J110" s="4"/>
       <c r="K110" s="4"/>
       <c r="L110" s="4"/>
+      <c r="M110" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
enny06 2019/09/02 14.00 Update print excel master item
</commit_message>
<xml_diff>
--- a/assets/templates/template_items_log.xlsx
+++ b/assets/templates/template_items_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\greebel\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A694BE9-AA92-4984-8C48-AF8236A29A17}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97E5C66-71C1-4FB7-950D-CEC093AD8387}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2D745729-4032-447E-85FB-C820FC51974E}"/>
   </bookViews>
@@ -121,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -158,6 +158,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,7 +484,7 @@
   <dimension ref="A1:O307"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E303" sqref="E303"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +523,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
+      <c r="I3" s="18"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
@@ -530,10 +539,10 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
+      <c r="I4" s="16"/>
       <c r="J4" s="11">
         <f ca="1">NOW()</f>
-        <v>43710.497383796297</v>
+        <v>43710.579024421299</v>
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
@@ -549,7 +558,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="I5" s="17"/>
       <c r="J5" s="8"/>
       <c r="K5" s="12"/>
       <c r="L5" s="8"/>
@@ -576,9 +585,9 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
enny06 2019/09/06 14.16 update print excel master item
</commit_message>
<xml_diff>
--- a/assets/templates/template_items_log.xlsx
+++ b/assets/templates/template_items_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\greebel\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97E5C66-71C1-4FB7-950D-CEC093AD8387}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7116A41-8DC3-409F-97BA-A69962EE84EA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2D745729-4032-447E-85FB-C820FC51974E}"/>
   </bookViews>
@@ -38,10 +38,10 @@
     <t>Item Code  :</t>
   </si>
   <si>
-    <t>Vendor   :</t>
+    <t>Vendor     :</t>
   </si>
   <si>
-    <t>Group     :</t>
+    <t>Group   :</t>
   </si>
 </sst>
 </file>
@@ -121,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -165,6 +165,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -481,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D347ED-B861-48B8-96B5-A98AF875B3CE}">
-  <dimension ref="A1:O307"/>
+  <dimension ref="A1:O376"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A373" workbookViewId="0">
+      <selection activeCell="N383" sqref="N383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,9 +526,9 @@
       <c r="C3" s="7"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
       <c r="I3" s="18"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
@@ -530,26 +536,23 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
       <c r="I4" s="16"/>
-      <c r="J4" s="11">
-        <f ca="1">NOW()</f>
-        <v>43710.579024421299</v>
-      </c>
+      <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
@@ -585,9 +588,10 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -604,6 +608,7 @@
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
@@ -619,6 +624,7 @@
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
@@ -634,6 +640,7 @@
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -649,6 +656,7 @@
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
@@ -664,6 +672,7 @@
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
       <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
@@ -679,6 +688,7 @@
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
@@ -694,6 +704,7 @@
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
       <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
@@ -709,6 +720,7 @@
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
       <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
@@ -724,8 +736,9 @@
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
       <c r="M16" s="14"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="14"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
@@ -739,8 +752,9 @@
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
       <c r="M17" s="14"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="14"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
@@ -754,8 +768,9 @@
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
       <c r="M18" s="14"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="14"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
@@ -769,8 +784,9 @@
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
       <c r="M19" s="14"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="14"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -784,8 +800,9 @@
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
       <c r="M20" s="14"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="14"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
@@ -799,8 +816,9 @@
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
       <c r="M21" s="14"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="14"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
@@ -814,8 +832,9 @@
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
       <c r="M22" s="14"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="14"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
@@ -829,8 +848,9 @@
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
       <c r="M23" s="14"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="14"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
@@ -844,8 +864,9 @@
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
       <c r="M24" s="14"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="14"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
@@ -859,8 +880,9 @@
       <c r="K25" s="14"/>
       <c r="L25" s="14"/>
       <c r="M25" s="14"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="14"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
@@ -874,8 +896,9 @@
       <c r="K26" s="14"/>
       <c r="L26" s="14"/>
       <c r="M26" s="14"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" s="14"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
@@ -889,8 +912,9 @@
       <c r="K27" s="14"/>
       <c r="L27" s="14"/>
       <c r="M27" s="14"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="14"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
@@ -904,8 +928,9 @@
       <c r="K28" s="14"/>
       <c r="L28" s="14"/>
       <c r="M28" s="14"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="14"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="5"/>
@@ -919,8 +944,9 @@
       <c r="K29" s="14"/>
       <c r="L29" s="14"/>
       <c r="M29" s="14"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" s="14"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
@@ -934,8 +960,9 @@
       <c r="K30" s="14"/>
       <c r="L30" s="14"/>
       <c r="M30" s="14"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30" s="14"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
@@ -949,8 +976,9 @@
       <c r="K31" s="14"/>
       <c r="L31" s="14"/>
       <c r="M31" s="14"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" s="14"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
@@ -964,8 +992,9 @@
       <c r="K32" s="14"/>
       <c r="L32" s="14"/>
       <c r="M32" s="14"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" s="14"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
@@ -979,8 +1008,9 @@
       <c r="K33" s="14"/>
       <c r="L33" s="14"/>
       <c r="M33" s="14"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" s="14"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
@@ -994,8 +1024,9 @@
       <c r="K34" s="14"/>
       <c r="L34" s="14"/>
       <c r="M34" s="14"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" s="14"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
@@ -1009,8 +1040,9 @@
       <c r="K35" s="14"/>
       <c r="L35" s="14"/>
       <c r="M35" s="14"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35" s="14"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
@@ -1024,8 +1056,9 @@
       <c r="K36" s="14"/>
       <c r="L36" s="14"/>
       <c r="M36" s="14"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36" s="14"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
@@ -1039,8 +1072,9 @@
       <c r="K37" s="14"/>
       <c r="L37" s="14"/>
       <c r="M37" s="14"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37" s="14"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="5"/>
@@ -1054,8 +1088,9 @@
       <c r="K38" s="14"/>
       <c r="L38" s="14"/>
       <c r="M38" s="14"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38" s="14"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
@@ -1069,8 +1104,9 @@
       <c r="K39" s="14"/>
       <c r="L39" s="14"/>
       <c r="M39" s="14"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39" s="14"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="5"/>
@@ -1084,8 +1120,9 @@
       <c r="K40" s="14"/>
       <c r="L40" s="14"/>
       <c r="M40" s="14"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40" s="14"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
@@ -1099,8 +1136,9 @@
       <c r="K41" s="14"/>
       <c r="L41" s="14"/>
       <c r="M41" s="14"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41" s="14"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="5"/>
@@ -1114,8 +1152,9 @@
       <c r="K42" s="14"/>
       <c r="L42" s="14"/>
       <c r="M42" s="14"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42" s="14"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="5"/>
@@ -1129,8 +1168,9 @@
       <c r="K43" s="14"/>
       <c r="L43" s="14"/>
       <c r="M43" s="14"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N43" s="14"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="5"/>
@@ -1144,8 +1184,9 @@
       <c r="K44" s="14"/>
       <c r="L44" s="14"/>
       <c r="M44" s="14"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N44" s="14"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="5"/>
@@ -1159,8 +1200,9 @@
       <c r="K45" s="14"/>
       <c r="L45" s="14"/>
       <c r="M45" s="14"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N45" s="14"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="E46" s="14"/>
@@ -1170,8 +1212,9 @@
       <c r="K46" s="15"/>
       <c r="L46" s="15"/>
       <c r="M46" s="14"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N46" s="14"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="E47" s="14"/>
@@ -1181,8 +1224,9 @@
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
       <c r="M47" s="14"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N47" s="14"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="E48" s="14"/>
@@ -1192,8 +1236,9 @@
       <c r="K48" s="15"/>
       <c r="L48" s="15"/>
       <c r="M48" s="14"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N48" s="14"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="E49" s="14"/>
@@ -1203,8 +1248,9 @@
       <c r="K49" s="15"/>
       <c r="L49" s="15"/>
       <c r="M49" s="14"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N49" s="14"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="E50" s="14"/>
@@ -1214,8 +1260,9 @@
       <c r="K50" s="15"/>
       <c r="L50" s="15"/>
       <c r="M50" s="14"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N50" s="14"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="E51" s="14"/>
@@ -1225,8 +1272,9 @@
       <c r="K51" s="15"/>
       <c r="L51" s="15"/>
       <c r="M51" s="14"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N51" s="14"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="E52" s="14"/>
@@ -1236,8 +1284,9 @@
       <c r="K52" s="15"/>
       <c r="L52" s="15"/>
       <c r="M52" s="14"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N52" s="14"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="E53" s="14"/>
@@ -1247,8 +1296,9 @@
       <c r="K53" s="15"/>
       <c r="L53" s="15"/>
       <c r="M53" s="14"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N53" s="14"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="E54" s="14"/>
@@ -1258,8 +1308,9 @@
       <c r="K54" s="15"/>
       <c r="L54" s="15"/>
       <c r="M54" s="14"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N54" s="14"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="E55" s="14"/>
@@ -1269,8 +1320,9 @@
       <c r="K55" s="15"/>
       <c r="L55" s="15"/>
       <c r="M55" s="14"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N55" s="14"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="E56" s="14"/>
@@ -1280,8 +1332,9 @@
       <c r="K56" s="15"/>
       <c r="L56" s="15"/>
       <c r="M56" s="14"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N56" s="14"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="E57" s="14"/>
@@ -1291,8 +1344,9 @@
       <c r="K57" s="15"/>
       <c r="L57" s="15"/>
       <c r="M57" s="14"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N57" s="14"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="E58" s="14"/>
@@ -1302,8 +1356,9 @@
       <c r="K58" s="15"/>
       <c r="L58" s="15"/>
       <c r="M58" s="14"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N58" s="14"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="E59" s="14"/>
@@ -1313,8 +1368,9 @@
       <c r="K59" s="15"/>
       <c r="L59" s="15"/>
       <c r="M59" s="14"/>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N59" s="14"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="E60" s="14"/>
@@ -1324,8 +1380,9 @@
       <c r="K60" s="15"/>
       <c r="L60" s="15"/>
       <c r="M60" s="14"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N60" s="14"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="E61" s="14"/>
@@ -1335,8 +1392,9 @@
       <c r="K61" s="15"/>
       <c r="L61" s="15"/>
       <c r="M61" s="14"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N61" s="14"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="E62" s="14"/>
@@ -1346,8 +1404,9 @@
       <c r="K62" s="15"/>
       <c r="L62" s="15"/>
       <c r="M62" s="14"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N62" s="14"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="E63" s="14"/>
@@ -1357,8 +1416,9 @@
       <c r="K63" s="15"/>
       <c r="L63" s="15"/>
       <c r="M63" s="14"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N63" s="14"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="E64" s="14"/>
@@ -1368,8 +1428,9 @@
       <c r="K64" s="15"/>
       <c r="L64" s="15"/>
       <c r="M64" s="14"/>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N64" s="14"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="E65" s="14"/>
       <c r="G65" s="15"/>
@@ -1378,8 +1439,9 @@
       <c r="K65" s="15"/>
       <c r="L65" s="15"/>
       <c r="M65" s="14"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N65" s="14"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="E66" s="14"/>
       <c r="G66" s="15"/>
@@ -1388,8 +1450,9 @@
       <c r="K66" s="15"/>
       <c r="L66" s="15"/>
       <c r="M66" s="14"/>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N66" s="14"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="E67" s="14"/>
       <c r="G67" s="15"/>
@@ -1398,8 +1461,9 @@
       <c r="K67" s="15"/>
       <c r="L67" s="15"/>
       <c r="M67" s="14"/>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N67" s="14"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="E68" s="14"/>
       <c r="G68" s="15"/>
@@ -1408,8 +1472,9 @@
       <c r="K68" s="15"/>
       <c r="L68" s="15"/>
       <c r="M68" s="14"/>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N68" s="14"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="E69" s="14"/>
       <c r="G69" s="15"/>
@@ -1418,8 +1483,9 @@
       <c r="K69" s="15"/>
       <c r="L69" s="15"/>
       <c r="M69" s="14"/>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N69" s="14"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="E70" s="14"/>
       <c r="G70" s="15"/>
@@ -1428,8 +1494,9 @@
       <c r="K70" s="15"/>
       <c r="L70" s="15"/>
       <c r="M70" s="14"/>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N70" s="14"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="E71" s="14"/>
       <c r="G71" s="15"/>
@@ -1438,8 +1505,9 @@
       <c r="K71" s="15"/>
       <c r="L71" s="15"/>
       <c r="M71" s="14"/>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N71" s="14"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="E72" s="14"/>
       <c r="G72" s="15"/>
@@ -1448,8 +1516,9 @@
       <c r="K72" s="15"/>
       <c r="L72" s="15"/>
       <c r="M72" s="14"/>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N72" s="14"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="E73" s="14"/>
       <c r="G73" s="15"/>
@@ -1458,8 +1527,9 @@
       <c r="K73" s="15"/>
       <c r="L73" s="15"/>
       <c r="M73" s="14"/>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N73" s="14"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="E74" s="14"/>
       <c r="G74" s="15"/>
@@ -1468,8 +1538,9 @@
       <c r="K74" s="15"/>
       <c r="L74" s="15"/>
       <c r="M74" s="14"/>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N74" s="14"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="E75" s="14"/>
       <c r="G75" s="15"/>
@@ -1478,8 +1549,9 @@
       <c r="K75" s="15"/>
       <c r="L75" s="15"/>
       <c r="M75" s="14"/>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N75" s="14"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="E76" s="14"/>
       <c r="G76" s="15"/>
@@ -1488,8 +1560,9 @@
       <c r="K76" s="15"/>
       <c r="L76" s="15"/>
       <c r="M76" s="14"/>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N76" s="14"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="E77" s="14"/>
       <c r="G77" s="15"/>
@@ -1498,8 +1571,9 @@
       <c r="K77" s="15"/>
       <c r="L77" s="15"/>
       <c r="M77" s="14"/>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N77" s="14"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="E78" s="14"/>
       <c r="G78" s="15"/>
@@ -1508,8 +1582,9 @@
       <c r="K78" s="15"/>
       <c r="L78" s="15"/>
       <c r="M78" s="14"/>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N78" s="14"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="E79" s="14"/>
       <c r="G79" s="15"/>
@@ -1518,8 +1593,9 @@
       <c r="K79" s="15"/>
       <c r="L79" s="15"/>
       <c r="M79" s="14"/>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N79" s="14"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="E80" s="14"/>
       <c r="G80" s="15"/>
@@ -1528,8 +1604,9 @@
       <c r="K80" s="15"/>
       <c r="L80" s="15"/>
       <c r="M80" s="14"/>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N80" s="14"/>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="E81" s="14"/>
       <c r="G81" s="15"/>
@@ -1538,8 +1615,9 @@
       <c r="K81" s="15"/>
       <c r="L81" s="15"/>
       <c r="M81" s="14"/>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N81" s="14"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="E82" s="14"/>
       <c r="G82" s="15"/>
@@ -1548,8 +1626,9 @@
       <c r="K82" s="15"/>
       <c r="L82" s="15"/>
       <c r="M82" s="14"/>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N82" s="14"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="E83" s="14"/>
       <c r="G83" s="15"/>
@@ -1558,8 +1637,9 @@
       <c r="K83" s="15"/>
       <c r="L83" s="15"/>
       <c r="M83" s="14"/>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N83" s="14"/>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="E84" s="14"/>
       <c r="G84" s="15"/>
@@ -1568,8 +1648,9 @@
       <c r="K84" s="15"/>
       <c r="L84" s="15"/>
       <c r="M84" s="14"/>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N84" s="14"/>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="E85" s="14"/>
       <c r="G85" s="15"/>
@@ -1578,8 +1659,9 @@
       <c r="K85" s="15"/>
       <c r="L85" s="15"/>
       <c r="M85" s="14"/>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N85" s="14"/>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="E86" s="14"/>
       <c r="G86" s="15"/>
@@ -1588,8 +1670,9 @@
       <c r="K86" s="15"/>
       <c r="L86" s="15"/>
       <c r="M86" s="14"/>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N86" s="14"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="E87" s="14"/>
       <c r="G87" s="15"/>
@@ -1598,8 +1681,9 @@
       <c r="K87" s="15"/>
       <c r="L87" s="15"/>
       <c r="M87" s="14"/>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N87" s="14"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="E88" s="14"/>
       <c r="G88" s="15"/>
@@ -1608,8 +1692,9 @@
       <c r="K88" s="15"/>
       <c r="L88" s="15"/>
       <c r="M88" s="14"/>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N88" s="14"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="E89" s="14"/>
       <c r="G89" s="15"/>
@@ -1618,8 +1703,9 @@
       <c r="K89" s="15"/>
       <c r="L89" s="15"/>
       <c r="M89" s="14"/>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N89" s="14"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="E90" s="14"/>
       <c r="G90" s="15"/>
@@ -1628,8 +1714,9 @@
       <c r="K90" s="15"/>
       <c r="L90" s="15"/>
       <c r="M90" s="14"/>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N90" s="14"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="E91" s="14"/>
       <c r="G91" s="15"/>
@@ -1638,8 +1725,9 @@
       <c r="K91" s="15"/>
       <c r="L91" s="15"/>
       <c r="M91" s="14"/>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N91" s="14"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="E92" s="14"/>
       <c r="G92" s="15"/>
@@ -1648,8 +1736,9 @@
       <c r="K92" s="15"/>
       <c r="L92" s="15"/>
       <c r="M92" s="14"/>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N92" s="14"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="E93" s="14"/>
       <c r="G93" s="15"/>
@@ -1658,8 +1747,9 @@
       <c r="K93" s="15"/>
       <c r="L93" s="15"/>
       <c r="M93" s="14"/>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N93" s="14"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="E94" s="14"/>
       <c r="G94" s="15"/>
@@ -1668,8 +1758,9 @@
       <c r="K94" s="15"/>
       <c r="L94" s="15"/>
       <c r="M94" s="14"/>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N94" s="14"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="E95" s="14"/>
       <c r="G95" s="15"/>
@@ -1678,8 +1769,9 @@
       <c r="K95" s="15"/>
       <c r="L95" s="15"/>
       <c r="M95" s="14"/>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N95" s="14"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="E96" s="14"/>
       <c r="G96" s="15"/>
@@ -1688,8 +1780,9 @@
       <c r="K96" s="15"/>
       <c r="L96" s="15"/>
       <c r="M96" s="14"/>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N96" s="14"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="E97" s="14"/>
       <c r="G97" s="15"/>
@@ -1698,8 +1791,9 @@
       <c r="K97" s="15"/>
       <c r="L97" s="15"/>
       <c r="M97" s="14"/>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N97" s="14"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="E98" s="14"/>
       <c r="G98" s="15"/>
@@ -1708,8 +1802,9 @@
       <c r="K98" s="15"/>
       <c r="L98" s="15"/>
       <c r="M98" s="14"/>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N98" s="14"/>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="E99" s="14"/>
       <c r="G99" s="15"/>
@@ -1718,8 +1813,9 @@
       <c r="K99" s="15"/>
       <c r="L99" s="15"/>
       <c r="M99" s="14"/>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N99" s="14"/>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="E100" s="14"/>
       <c r="G100" s="15"/>
@@ -1728,8 +1824,9 @@
       <c r="K100" s="15"/>
       <c r="L100" s="15"/>
       <c r="M100" s="14"/>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N100" s="14"/>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="E101" s="14"/>
       <c r="G101" s="15"/>
@@ -1738,8 +1835,9 @@
       <c r="K101" s="15"/>
       <c r="L101" s="15"/>
       <c r="M101" s="14"/>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N101" s="14"/>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="E102" s="14"/>
       <c r="G102" s="15"/>
@@ -1748,8 +1846,9 @@
       <c r="K102" s="15"/>
       <c r="L102" s="15"/>
       <c r="M102" s="14"/>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N102" s="14"/>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="E103" s="14"/>
       <c r="G103" s="15"/>
@@ -1758,8 +1857,9 @@
       <c r="K103" s="15"/>
       <c r="L103" s="15"/>
       <c r="M103" s="14"/>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N103" s="14"/>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="E104" s="14"/>
       <c r="G104" s="15"/>
@@ -1768,8 +1868,9 @@
       <c r="K104" s="15"/>
       <c r="L104" s="15"/>
       <c r="M104" s="14"/>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N104" s="14"/>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="E105" s="14"/>
       <c r="G105" s="15"/>
@@ -1778,8 +1879,9 @@
       <c r="K105" s="15"/>
       <c r="L105" s="15"/>
       <c r="M105" s="14"/>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N105" s="14"/>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="E106" s="14"/>
       <c r="G106" s="15"/>
@@ -1788,8 +1890,9 @@
       <c r="K106" s="15"/>
       <c r="L106" s="15"/>
       <c r="M106" s="14"/>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N106" s="14"/>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="E107" s="14"/>
       <c r="G107" s="15"/>
@@ -1798,8 +1901,9 @@
       <c r="K107" s="15"/>
       <c r="L107" s="15"/>
       <c r="M107" s="14"/>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N107" s="14"/>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E108" s="14"/>
       <c r="G108" s="15"/>
       <c r="I108" s="15"/>
@@ -1807,8 +1911,9 @@
       <c r="K108" s="15"/>
       <c r="L108" s="15"/>
       <c r="M108" s="14"/>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N108" s="14"/>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E109" s="14"/>
       <c r="G109" s="15"/>
       <c r="I109" s="15"/>
@@ -1816,8 +1921,9 @@
       <c r="K109" s="15"/>
       <c r="L109" s="15"/>
       <c r="M109" s="14"/>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N109" s="14"/>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E110" s="14"/>
       <c r="G110" s="15"/>
       <c r="I110" s="15"/>
@@ -1825,8 +1931,9 @@
       <c r="K110" s="15"/>
       <c r="L110" s="15"/>
       <c r="M110" s="14"/>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N110" s="14"/>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E111" s="14"/>
       <c r="G111" s="15"/>
       <c r="I111" s="15"/>
@@ -1834,8 +1941,9 @@
       <c r="K111" s="15"/>
       <c r="L111" s="15"/>
       <c r="M111" s="15"/>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N111" s="14"/>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E112" s="14"/>
       <c r="G112" s="15"/>
       <c r="I112" s="15"/>
@@ -1843,8 +1951,9 @@
       <c r="K112" s="15"/>
       <c r="L112" s="15"/>
       <c r="M112" s="15"/>
-    </row>
-    <row r="113" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N112" s="14"/>
+    </row>
+    <row r="113" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E113" s="14"/>
       <c r="G113" s="15"/>
       <c r="I113" s="15"/>
@@ -1852,8 +1961,9 @@
       <c r="K113" s="15"/>
       <c r="L113" s="15"/>
       <c r="M113" s="15"/>
-    </row>
-    <row r="114" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N113" s="14"/>
+    </row>
+    <row r="114" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E114" s="14"/>
       <c r="G114" s="15"/>
       <c r="I114" s="15"/>
@@ -1861,8 +1971,9 @@
       <c r="K114" s="15"/>
       <c r="L114" s="15"/>
       <c r="M114" s="15"/>
-    </row>
-    <row r="115" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N114" s="14"/>
+    </row>
+    <row r="115" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E115" s="14"/>
       <c r="G115" s="15"/>
       <c r="I115" s="15"/>
@@ -1870,642 +1981,1042 @@
       <c r="K115" s="15"/>
       <c r="L115" s="15"/>
       <c r="M115" s="15"/>
-    </row>
-    <row r="116" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N115" s="14"/>
+    </row>
+    <row r="116" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E116" s="14"/>
       <c r="I116" s="15"/>
       <c r="J116" s="15"/>
       <c r="K116" s="15"/>
       <c r="L116" s="15"/>
       <c r="M116" s="15"/>
-    </row>
-    <row r="117" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N116" s="14"/>
+    </row>
+    <row r="117" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E117" s="14"/>
       <c r="I117" s="15"/>
       <c r="J117" s="15"/>
       <c r="K117" s="15"/>
       <c r="L117" s="15"/>
       <c r="M117" s="15"/>
-    </row>
-    <row r="118" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N117" s="14"/>
+    </row>
+    <row r="118" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E118" s="14"/>
       <c r="I118" s="15"/>
       <c r="J118" s="15"/>
       <c r="K118" s="15"/>
       <c r="L118" s="15"/>
       <c r="M118" s="15"/>
-    </row>
-    <row r="119" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N118" s="14"/>
+    </row>
+    <row r="119" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E119" s="14"/>
       <c r="I119" s="15"/>
       <c r="J119" s="15"/>
       <c r="K119" s="15"/>
       <c r="L119" s="15"/>
       <c r="M119" s="15"/>
-    </row>
-    <row r="120" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N119" s="14"/>
+    </row>
+    <row r="120" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E120" s="14"/>
       <c r="I120" s="15"/>
       <c r="J120" s="15"/>
       <c r="K120" s="15"/>
       <c r="L120" s="15"/>
       <c r="M120" s="15"/>
-    </row>
-    <row r="121" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N120" s="14"/>
+    </row>
+    <row r="121" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E121" s="14"/>
       <c r="I121" s="15"/>
       <c r="J121" s="15"/>
       <c r="K121" s="15"/>
       <c r="L121" s="15"/>
       <c r="M121" s="15"/>
-    </row>
-    <row r="122" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N121" s="14"/>
+    </row>
+    <row r="122" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E122" s="14"/>
       <c r="I122" s="15"/>
       <c r="J122" s="15"/>
       <c r="K122" s="15"/>
       <c r="L122" s="15"/>
       <c r="M122" s="15"/>
-    </row>
-    <row r="123" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N122" s="14"/>
+    </row>
+    <row r="123" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E123" s="14"/>
       <c r="I123" s="15"/>
       <c r="J123" s="15"/>
       <c r="K123" s="15"/>
       <c r="L123" s="15"/>
       <c r="M123" s="15"/>
-    </row>
-    <row r="124" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N123" s="14"/>
+    </row>
+    <row r="124" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E124" s="14"/>
       <c r="I124" s="15"/>
       <c r="J124" s="15"/>
       <c r="K124" s="15"/>
       <c r="L124" s="15"/>
       <c r="M124" s="15"/>
-    </row>
-    <row r="125" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N124" s="14"/>
+    </row>
+    <row r="125" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E125" s="14"/>
       <c r="I125" s="15"/>
       <c r="J125" s="15"/>
       <c r="K125" s="15"/>
       <c r="L125" s="15"/>
       <c r="M125" s="15"/>
-    </row>
-    <row r="126" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N125" s="14"/>
+    </row>
+    <row r="126" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E126" s="14"/>
       <c r="I126" s="15"/>
       <c r="J126" s="15"/>
       <c r="K126" s="15"/>
       <c r="L126" s="15"/>
       <c r="M126" s="15"/>
-    </row>
-    <row r="127" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N126" s="14"/>
+    </row>
+    <row r="127" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E127" s="14"/>
       <c r="I127" s="15"/>
       <c r="J127" s="15"/>
       <c r="K127" s="15"/>
       <c r="L127" s="15"/>
       <c r="M127" s="15"/>
-    </row>
-    <row r="128" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="N127" s="14"/>
+    </row>
+    <row r="128" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E128" s="14"/>
-    </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N128" s="14"/>
+    </row>
+    <row r="129" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E129" s="14"/>
-    </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N129" s="14"/>
+    </row>
+    <row r="130" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E130" s="14"/>
-    </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N130" s="14"/>
+    </row>
+    <row r="131" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E131" s="14"/>
-    </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N131" s="14"/>
+    </row>
+    <row r="132" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E132" s="14"/>
-    </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N132" s="14"/>
+    </row>
+    <row r="133" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E133" s="14"/>
-    </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N133" s="14"/>
+    </row>
+    <row r="134" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E134" s="14"/>
-    </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N134" s="14"/>
+    </row>
+    <row r="135" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E135" s="14"/>
-    </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N135" s="14"/>
+    </row>
+    <row r="136" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E136" s="14"/>
-    </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N136" s="14"/>
+    </row>
+    <row r="137" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E137" s="14"/>
-    </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N137" s="14"/>
+    </row>
+    <row r="138" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E138" s="14"/>
-    </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N138" s="14"/>
+    </row>
+    <row r="139" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E139" s="14"/>
-    </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N139" s="14"/>
+    </row>
+    <row r="140" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E140" s="14"/>
-    </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N140" s="14"/>
+    </row>
+    <row r="141" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E141" s="14"/>
-    </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N141" s="14"/>
+    </row>
+    <row r="142" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E142" s="14"/>
-    </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N142" s="14"/>
+    </row>
+    <row r="143" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E143" s="14"/>
-    </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N143" s="14"/>
+    </row>
+    <row r="144" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E144" s="14"/>
-    </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N144" s="14"/>
+    </row>
+    <row r="145" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E145" s="14"/>
-    </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N145" s="14"/>
+    </row>
+    <row r="146" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E146" s="14"/>
-    </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N146" s="14"/>
+    </row>
+    <row r="147" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E147" s="14"/>
-    </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N147" s="14"/>
+    </row>
+    <row r="148" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E148" s="14"/>
-    </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N148" s="14"/>
+    </row>
+    <row r="149" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E149" s="14"/>
-    </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N149" s="14"/>
+    </row>
+    <row r="150" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E150" s="14"/>
-    </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N150" s="14"/>
+    </row>
+    <row r="151" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E151" s="14"/>
-    </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N151" s="14"/>
+    </row>
+    <row r="152" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E152" s="14"/>
-    </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N152" s="14"/>
+    </row>
+    <row r="153" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E153" s="14"/>
-    </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N153" s="14"/>
+    </row>
+    <row r="154" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E154" s="14"/>
-    </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N154" s="14"/>
+    </row>
+    <row r="155" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E155" s="14"/>
-    </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N155" s="14"/>
+    </row>
+    <row r="156" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E156" s="14"/>
-    </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N156" s="14"/>
+    </row>
+    <row r="157" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E157" s="14"/>
-    </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N157" s="14"/>
+    </row>
+    <row r="158" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E158" s="14"/>
-    </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N158" s="14"/>
+    </row>
+    <row r="159" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E159" s="14"/>
-    </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N159" s="14"/>
+    </row>
+    <row r="160" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E160" s="14"/>
-    </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N160" s="14"/>
+    </row>
+    <row r="161" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E161" s="14"/>
-    </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N161" s="14"/>
+    </row>
+    <row r="162" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E162" s="14"/>
-    </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N162" s="14"/>
+    </row>
+    <row r="163" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E163" s="14"/>
-    </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N163" s="14"/>
+    </row>
+    <row r="164" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E164" s="14"/>
-    </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N164" s="14"/>
+    </row>
+    <row r="165" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E165" s="14"/>
-    </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N165" s="14"/>
+    </row>
+    <row r="166" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E166" s="14"/>
-    </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N166" s="14"/>
+    </row>
+    <row r="167" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E167" s="14"/>
-    </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N167" s="14"/>
+    </row>
+    <row r="168" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E168" s="14"/>
-    </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N168" s="14"/>
+    </row>
+    <row r="169" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E169" s="14"/>
-    </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N169" s="14"/>
+    </row>
+    <row r="170" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E170" s="14"/>
-    </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N170" s="14"/>
+    </row>
+    <row r="171" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E171" s="14"/>
-    </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N171" s="14"/>
+    </row>
+    <row r="172" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E172" s="14"/>
-    </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N172" s="14"/>
+    </row>
+    <row r="173" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E173" s="14"/>
-    </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N173" s="14"/>
+    </row>
+    <row r="174" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E174" s="14"/>
-    </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N174" s="14"/>
+    </row>
+    <row r="175" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E175" s="14"/>
-    </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N175" s="14"/>
+    </row>
+    <row r="176" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E176" s="14"/>
-    </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N176" s="14"/>
+    </row>
+    <row r="177" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E177" s="14"/>
-    </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N177" s="14"/>
+    </row>
+    <row r="178" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E178" s="14"/>
-    </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N178" s="14"/>
+    </row>
+    <row r="179" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E179" s="14"/>
-    </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N179" s="14"/>
+    </row>
+    <row r="180" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E180" s="14"/>
-    </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N180" s="14"/>
+    </row>
+    <row r="181" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E181" s="14"/>
-    </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N181" s="14"/>
+    </row>
+    <row r="182" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E182" s="14"/>
-    </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N182" s="14"/>
+    </row>
+    <row r="183" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E183" s="14"/>
-    </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N183" s="14"/>
+    </row>
+    <row r="184" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E184" s="14"/>
-    </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N184" s="14"/>
+    </row>
+    <row r="185" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E185" s="14"/>
-    </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N185" s="14"/>
+    </row>
+    <row r="186" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E186" s="14"/>
-    </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N186" s="14"/>
+    </row>
+    <row r="187" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E187" s="14"/>
-    </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N187" s="14"/>
+    </row>
+    <row r="188" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E188" s="14"/>
-    </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N188" s="14"/>
+    </row>
+    <row r="189" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E189" s="14"/>
-    </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N189" s="14"/>
+    </row>
+    <row r="190" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E190" s="14"/>
-    </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N190" s="14"/>
+    </row>
+    <row r="191" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E191" s="14"/>
-    </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N191" s="14"/>
+    </row>
+    <row r="192" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E192" s="14"/>
-    </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N192" s="14"/>
+    </row>
+    <row r="193" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E193" s="14"/>
-    </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N193" s="14"/>
+    </row>
+    <row r="194" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E194" s="14"/>
-    </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N194" s="14"/>
+    </row>
+    <row r="195" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E195" s="14"/>
-    </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N195" s="14"/>
+    </row>
+    <row r="196" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E196" s="14"/>
-    </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N196" s="14"/>
+    </row>
+    <row r="197" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E197" s="14"/>
-    </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N197" s="14"/>
+    </row>
+    <row r="198" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E198" s="14"/>
-    </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N198" s="14"/>
+    </row>
+    <row r="199" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E199" s="14"/>
-    </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N199" s="14"/>
+    </row>
+    <row r="200" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E200" s="14"/>
-    </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N200" s="14"/>
+    </row>
+    <row r="201" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E201" s="14"/>
-    </row>
-    <row r="202" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N201" s="14"/>
+    </row>
+    <row r="202" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E202" s="14"/>
-    </row>
-    <row r="203" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N202" s="14"/>
+    </row>
+    <row r="203" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E203" s="14"/>
-    </row>
-    <row r="204" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N203" s="14"/>
+    </row>
+    <row r="204" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E204" s="14"/>
-    </row>
-    <row r="205" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N204" s="14"/>
+    </row>
+    <row r="205" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E205" s="14"/>
-    </row>
-    <row r="206" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N205" s="14"/>
+    </row>
+    <row r="206" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E206" s="14"/>
-    </row>
-    <row r="207" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N206" s="14"/>
+    </row>
+    <row r="207" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E207" s="14"/>
-    </row>
-    <row r="208" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N207" s="14"/>
+    </row>
+    <row r="208" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E208" s="14"/>
-    </row>
-    <row r="209" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N208" s="14"/>
+    </row>
+    <row r="209" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E209" s="14"/>
-    </row>
-    <row r="210" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N209" s="14"/>
+    </row>
+    <row r="210" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E210" s="14"/>
-    </row>
-    <row r="211" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N210" s="14"/>
+    </row>
+    <row r="211" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E211" s="14"/>
-    </row>
-    <row r="212" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N211" s="14"/>
+    </row>
+    <row r="212" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E212" s="14"/>
-    </row>
-    <row r="213" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N212" s="14"/>
+    </row>
+    <row r="213" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E213" s="14"/>
-    </row>
-    <row r="214" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N213" s="14"/>
+    </row>
+    <row r="214" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E214" s="14"/>
-    </row>
-    <row r="215" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N214" s="14"/>
+    </row>
+    <row r="215" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E215" s="14"/>
-    </row>
-    <row r="216" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N215" s="14"/>
+    </row>
+    <row r="216" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E216" s="14"/>
-    </row>
-    <row r="217" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N216" s="14"/>
+    </row>
+    <row r="217" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E217" s="14"/>
-    </row>
-    <row r="218" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N217" s="14"/>
+    </row>
+    <row r="218" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E218" s="14"/>
-    </row>
-    <row r="219" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N218" s="14"/>
+    </row>
+    <row r="219" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E219" s="14"/>
-    </row>
-    <row r="220" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N219" s="14"/>
+    </row>
+    <row r="220" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E220" s="14"/>
-    </row>
-    <row r="221" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N220" s="14"/>
+    </row>
+    <row r="221" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E221" s="14"/>
-    </row>
-    <row r="222" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N221" s="14"/>
+    </row>
+    <row r="222" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E222" s="14"/>
-    </row>
-    <row r="223" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N222" s="14"/>
+    </row>
+    <row r="223" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E223" s="14"/>
-    </row>
-    <row r="224" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N223" s="14"/>
+    </row>
+    <row r="224" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E224" s="14"/>
-    </row>
-    <row r="225" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N224" s="14"/>
+    </row>
+    <row r="225" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E225" s="14"/>
-    </row>
-    <row r="226" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N225" s="14"/>
+    </row>
+    <row r="226" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E226" s="14"/>
-    </row>
-    <row r="227" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N226" s="14"/>
+    </row>
+    <row r="227" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E227" s="14"/>
-    </row>
-    <row r="228" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N227" s="14"/>
+    </row>
+    <row r="228" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E228" s="14"/>
-    </row>
-    <row r="229" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N228" s="14"/>
+    </row>
+    <row r="229" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E229" s="14"/>
-    </row>
-    <row r="230" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N229" s="14"/>
+    </row>
+    <row r="230" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E230" s="14"/>
-    </row>
-    <row r="231" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N230" s="14"/>
+    </row>
+    <row r="231" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E231" s="14"/>
-    </row>
-    <row r="232" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N231" s="14"/>
+    </row>
+    <row r="232" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E232" s="14"/>
-    </row>
-    <row r="233" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N232" s="14"/>
+    </row>
+    <row r="233" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E233" s="14"/>
-    </row>
-    <row r="234" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N233" s="14"/>
+    </row>
+    <row r="234" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E234" s="14"/>
-    </row>
-    <row r="235" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N234" s="14"/>
+    </row>
+    <row r="235" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E235" s="14"/>
-    </row>
-    <row r="236" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N235" s="14"/>
+    </row>
+    <row r="236" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E236" s="14"/>
-    </row>
-    <row r="237" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N236" s="14"/>
+    </row>
+    <row r="237" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E237" s="14"/>
-    </row>
-    <row r="238" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N237" s="14"/>
+    </row>
+    <row r="238" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E238" s="14"/>
-    </row>
-    <row r="239" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N238" s="14"/>
+    </row>
+    <row r="239" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E239" s="14"/>
-    </row>
-    <row r="240" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N239" s="14"/>
+    </row>
+    <row r="240" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E240" s="14"/>
-    </row>
-    <row r="241" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N240" s="14"/>
+    </row>
+    <row r="241" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E241" s="14"/>
-    </row>
-    <row r="242" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N241" s="14"/>
+    </row>
+    <row r="242" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E242" s="14"/>
-    </row>
-    <row r="243" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N242" s="14"/>
+    </row>
+    <row r="243" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E243" s="14"/>
-    </row>
-    <row r="244" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N243" s="14"/>
+    </row>
+    <row r="244" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E244" s="14"/>
-    </row>
-    <row r="245" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N244" s="14"/>
+    </row>
+    <row r="245" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E245" s="14"/>
-    </row>
-    <row r="246" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N245" s="14"/>
+    </row>
+    <row r="246" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E246" s="14"/>
-    </row>
-    <row r="247" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N246" s="14"/>
+    </row>
+    <row r="247" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E247" s="14"/>
-    </row>
-    <row r="248" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N247" s="14"/>
+    </row>
+    <row r="248" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E248" s="14"/>
-    </row>
-    <row r="249" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N248" s="14"/>
+    </row>
+    <row r="249" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E249" s="14"/>
-    </row>
-    <row r="250" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N249" s="14"/>
+    </row>
+    <row r="250" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E250" s="14"/>
-    </row>
-    <row r="251" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N250" s="14"/>
+    </row>
+    <row r="251" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E251" s="14"/>
-    </row>
-    <row r="252" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N251" s="14"/>
+    </row>
+    <row r="252" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E252" s="14"/>
-    </row>
-    <row r="253" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N252" s="14"/>
+    </row>
+    <row r="253" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E253" s="14"/>
-    </row>
-    <row r="254" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N253" s="14"/>
+    </row>
+    <row r="254" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E254" s="14"/>
-    </row>
-    <row r="255" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N254" s="14"/>
+    </row>
+    <row r="255" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E255" s="14"/>
-    </row>
-    <row r="256" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N255" s="14"/>
+    </row>
+    <row r="256" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E256" s="14"/>
-    </row>
-    <row r="257" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N256" s="14"/>
+    </row>
+    <row r="257" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E257" s="14"/>
-    </row>
-    <row r="258" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N257" s="14"/>
+    </row>
+    <row r="258" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E258" s="14"/>
-    </row>
-    <row r="259" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N258" s="14"/>
+    </row>
+    <row r="259" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E259" s="14"/>
-    </row>
-    <row r="260" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N259" s="14"/>
+    </row>
+    <row r="260" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E260" s="14"/>
-    </row>
-    <row r="261" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N260" s="14"/>
+    </row>
+    <row r="261" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E261" s="14"/>
-    </row>
-    <row r="262" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N261" s="14"/>
+    </row>
+    <row r="262" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E262" s="14"/>
-    </row>
-    <row r="263" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N262" s="14"/>
+    </row>
+    <row r="263" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E263" s="14"/>
-    </row>
-    <row r="264" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N263" s="14"/>
+    </row>
+    <row r="264" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E264" s="14"/>
-    </row>
-    <row r="265" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N264" s="14"/>
+    </row>
+    <row r="265" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E265" s="14"/>
-    </row>
-    <row r="266" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N265" s="14"/>
+    </row>
+    <row r="266" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E266" s="14"/>
-    </row>
-    <row r="267" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N266" s="14"/>
+    </row>
+    <row r="267" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E267" s="14"/>
-    </row>
-    <row r="268" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N267" s="14"/>
+    </row>
+    <row r="268" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E268" s="14"/>
-    </row>
-    <row r="269" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N268" s="14"/>
+    </row>
+    <row r="269" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E269" s="14"/>
-    </row>
-    <row r="270" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N269" s="14"/>
+    </row>
+    <row r="270" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E270" s="14"/>
-    </row>
-    <row r="271" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N270" s="14"/>
+    </row>
+    <row r="271" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E271" s="14"/>
-    </row>
-    <row r="272" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N271" s="14"/>
+    </row>
+    <row r="272" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E272" s="14"/>
-    </row>
-    <row r="273" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N272" s="14"/>
+    </row>
+    <row r="273" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E273" s="14"/>
-    </row>
-    <row r="274" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N273" s="14"/>
+    </row>
+    <row r="274" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E274" s="14"/>
-    </row>
-    <row r="275" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N274" s="14"/>
+    </row>
+    <row r="275" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E275" s="14"/>
-    </row>
-    <row r="276" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N275" s="14"/>
+    </row>
+    <row r="276" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E276" s="14"/>
-    </row>
-    <row r="277" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N276" s="14"/>
+    </row>
+    <row r="277" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E277" s="14"/>
-    </row>
-    <row r="278" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N277" s="14"/>
+    </row>
+    <row r="278" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E278" s="14"/>
-    </row>
-    <row r="279" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N278" s="14"/>
+    </row>
+    <row r="279" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E279" s="14"/>
-    </row>
-    <row r="280" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N279" s="14"/>
+    </row>
+    <row r="280" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E280" s="14"/>
-    </row>
-    <row r="281" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N280" s="14"/>
+    </row>
+    <row r="281" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E281" s="14"/>
-    </row>
-    <row r="282" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N281" s="14"/>
+    </row>
+    <row r="282" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E282" s="14"/>
-    </row>
-    <row r="283" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N282" s="14"/>
+    </row>
+    <row r="283" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E283" s="14"/>
-    </row>
-    <row r="284" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N283" s="14"/>
+    </row>
+    <row r="284" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E284" s="14"/>
-    </row>
-    <row r="285" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N284" s="14"/>
+    </row>
+    <row r="285" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E285" s="14"/>
-    </row>
-    <row r="286" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N285" s="14"/>
+    </row>
+    <row r="286" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E286" s="14"/>
-    </row>
-    <row r="287" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N286" s="14"/>
+    </row>
+    <row r="287" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E287" s="14"/>
-    </row>
-    <row r="288" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N287" s="14"/>
+    </row>
+    <row r="288" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E288" s="14"/>
-    </row>
-    <row r="289" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N288" s="14"/>
+    </row>
+    <row r="289" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E289" s="14"/>
-    </row>
-    <row r="290" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N289" s="14"/>
+    </row>
+    <row r="290" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E290" s="14"/>
-    </row>
-    <row r="291" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N290" s="14"/>
+    </row>
+    <row r="291" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E291" s="14"/>
-    </row>
-    <row r="292" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N291" s="14"/>
+    </row>
+    <row r="292" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E292" s="14"/>
-    </row>
-    <row r="293" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N292" s="14"/>
+    </row>
+    <row r="293" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E293" s="14"/>
-    </row>
-    <row r="294" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N293" s="14"/>
+    </row>
+    <row r="294" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E294" s="14"/>
-    </row>
-    <row r="295" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N294" s="14"/>
+    </row>
+    <row r="295" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E295" s="14"/>
-    </row>
-    <row r="296" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N295" s="14"/>
+    </row>
+    <row r="296" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E296" s="14"/>
-    </row>
-    <row r="297" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N296" s="14"/>
+    </row>
+    <row r="297" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E297" s="14"/>
-    </row>
-    <row r="298" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N297" s="14"/>
+    </row>
+    <row r="298" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E298" s="14"/>
-    </row>
-    <row r="299" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N298" s="14"/>
+    </row>
+    <row r="299" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E299" s="14"/>
-    </row>
-    <row r="300" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N299" s="14"/>
+    </row>
+    <row r="300" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E300" s="14"/>
-    </row>
-    <row r="301" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N300" s="14"/>
+    </row>
+    <row r="301" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E301" s="14"/>
-    </row>
-    <row r="302" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N301" s="14"/>
+    </row>
+    <row r="302" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E302" s="14"/>
-    </row>
-    <row r="303" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N302" s="14"/>
+    </row>
+    <row r="303" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E303" s="14"/>
-    </row>
-    <row r="304" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N303" s="14"/>
+    </row>
+    <row r="304" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E304" s="14"/>
-    </row>
-    <row r="305" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N304" s="14"/>
+    </row>
+    <row r="305" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E305" s="14"/>
-    </row>
-    <row r="306" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N305" s="14"/>
+    </row>
+    <row r="306" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E306" s="14"/>
-    </row>
-    <row r="307" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="N306" s="14"/>
+    </row>
+    <row r="307" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E307" s="14"/>
+      <c r="N307" s="14"/>
+    </row>
+    <row r="308" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N308" s="14"/>
+    </row>
+    <row r="309" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N309" s="14"/>
+    </row>
+    <row r="310" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N310" s="14"/>
+    </row>
+    <row r="311" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N311" s="14"/>
+    </row>
+    <row r="312" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N312" s="14"/>
+    </row>
+    <row r="313" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N313" s="14"/>
+    </row>
+    <row r="314" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N314" s="14"/>
+    </row>
+    <row r="315" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N315" s="14"/>
+    </row>
+    <row r="316" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N316" s="14"/>
+    </row>
+    <row r="317" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N317" s="14"/>
+    </row>
+    <row r="318" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N318" s="14"/>
+    </row>
+    <row r="319" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N319" s="14"/>
+    </row>
+    <row r="320" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="N320" s="14"/>
+    </row>
+    <row r="321" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N321" s="14"/>
+    </row>
+    <row r="322" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N322" s="14"/>
+    </row>
+    <row r="323" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N323" s="14"/>
+    </row>
+    <row r="324" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N324" s="14"/>
+    </row>
+    <row r="325" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N325" s="14"/>
+    </row>
+    <row r="326" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N326" s="14"/>
+    </row>
+    <row r="327" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N327" s="14"/>
+    </row>
+    <row r="328" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N328" s="14"/>
+    </row>
+    <row r="329" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N329" s="14"/>
+    </row>
+    <row r="330" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N330" s="14"/>
+    </row>
+    <row r="331" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N331" s="14"/>
+    </row>
+    <row r="332" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N332" s="14"/>
+    </row>
+    <row r="333" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N333" s="14"/>
+    </row>
+    <row r="334" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N334" s="14"/>
+    </row>
+    <row r="335" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N335" s="14"/>
+    </row>
+    <row r="336" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N336" s="14"/>
+    </row>
+    <row r="337" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N337" s="14"/>
+    </row>
+    <row r="338" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N338" s="14"/>
+    </row>
+    <row r="339" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N339" s="14"/>
+    </row>
+    <row r="340" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N340" s="14"/>
+    </row>
+    <row r="341" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N341" s="14"/>
+    </row>
+    <row r="342" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N342" s="14"/>
+    </row>
+    <row r="343" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N343" s="14"/>
+    </row>
+    <row r="344" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N344" s="14"/>
+    </row>
+    <row r="345" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N345" s="14"/>
+    </row>
+    <row r="346" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N346" s="14"/>
+    </row>
+    <row r="347" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N347" s="14"/>
+    </row>
+    <row r="348" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N348" s="14"/>
+    </row>
+    <row r="349" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N349" s="14"/>
+    </row>
+    <row r="350" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N350" s="14"/>
+    </row>
+    <row r="351" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N351" s="14"/>
+    </row>
+    <row r="352" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N352" s="14"/>
+    </row>
+    <row r="353" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N353" s="14"/>
+    </row>
+    <row r="354" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N354" s="14"/>
+    </row>
+    <row r="355" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N355" s="14"/>
+    </row>
+    <row r="356" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N356" s="14"/>
+    </row>
+    <row r="357" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N357" s="14"/>
+    </row>
+    <row r="358" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N358" s="14"/>
+    </row>
+    <row r="359" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N359" s="14"/>
+    </row>
+    <row r="360" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N360" s="14"/>
+    </row>
+    <row r="361" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N361" s="14"/>
+    </row>
+    <row r="362" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N362" s="14"/>
+    </row>
+    <row r="363" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N363" s="14"/>
+    </row>
+    <row r="364" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N364" s="14"/>
+    </row>
+    <row r="365" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N365" s="14"/>
+    </row>
+    <row r="366" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N366" s="14"/>
+    </row>
+    <row r="367" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N367" s="14"/>
+    </row>
+    <row r="368" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N368" s="14"/>
+    </row>
+    <row r="369" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N369" s="14"/>
+    </row>
+    <row r="370" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N370" s="14"/>
+    </row>
+    <row r="371" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N371" s="14"/>
+    </row>
+    <row r="372" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N372" s="14"/>
+    </row>
+    <row r="373" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N373" s="14"/>
+    </row>
+    <row r="374" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N374" s="14"/>
+    </row>
+    <row r="375" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N375" s="14"/>
+    </row>
+    <row r="376" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N376" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
enny06 17/09/2019 18.18 Update master item print excel
</commit_message>
<xml_diff>
--- a/assets/templates/template_items_log.xlsx
+++ b/assets/templates/template_items_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\greebel\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7116A41-8DC3-409F-97BA-A69962EE84EA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79A6BF0-42B5-4ECA-9693-9DE8D5DB99D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2D745729-4032-447E-85FB-C820FC51974E}"/>
   </bookViews>
@@ -32,9 +32,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Awal s/d Akhir</t>
-  </si>
-  <si>
     <t>Item Code  :</t>
   </si>
   <si>
@@ -42,6 +39,9 @@
   </si>
   <si>
     <t>Group   :</t>
+  </si>
+  <si>
+    <t>Awal  s/d  Akhir</t>
   </si>
 </sst>
 </file>
@@ -121,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -173,6 +173,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D347ED-B861-48B8-96B5-A98AF875B3CE}">
-  <dimension ref="A1:O376"/>
+  <dimension ref="A1:O455"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A373" workbookViewId="0">
-      <selection activeCell="N383" sqref="N383"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,10 +521,10 @@
     </row>
     <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="9"/>
@@ -533,10 +536,12 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
@@ -552,7 +557,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
@@ -601,14 +606,14 @@
       <c r="D8" s="5"/>
       <c r="E8" s="14"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="14"/>
+      <c r="G8" s="22"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
@@ -617,7 +622,7 @@
       <c r="D9" s="5"/>
       <c r="E9" s="14"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="14"/>
+      <c r="G9" s="22"/>
       <c r="H9" s="5"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
@@ -633,7 +638,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="14"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="14"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="5"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
@@ -649,7 +654,7 @@
       <c r="D11" s="5"/>
       <c r="E11" s="14"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="14"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="5"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -665,7 +670,7 @@
       <c r="D12" s="5"/>
       <c r="E12" s="14"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="14"/>
+      <c r="G12" s="22"/>
       <c r="H12" s="5"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
@@ -681,7 +686,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="14"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="14"/>
+      <c r="G13" s="22"/>
       <c r="H13" s="5"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
@@ -697,7 +702,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="14"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="14"/>
+      <c r="G14" s="22"/>
       <c r="H14" s="5"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -713,7 +718,7 @@
       <c r="D15" s="5"/>
       <c r="E15" s="14"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="14"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="5"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
@@ -729,7 +734,7 @@
       <c r="D16" s="5"/>
       <c r="E16" s="14"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="14"/>
+      <c r="G16" s="22"/>
       <c r="H16" s="5"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
@@ -745,7 +750,7 @@
       <c r="D17" s="5"/>
       <c r="E17" s="14"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="14"/>
+      <c r="G17" s="22"/>
       <c r="H17" s="5"/>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
@@ -761,7 +766,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="14"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="14"/>
+      <c r="G18" s="22"/>
       <c r="H18" s="5"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -777,7 +782,7 @@
       <c r="D19" s="5"/>
       <c r="E19" s="14"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="14"/>
+      <c r="G19" s="22"/>
       <c r="H19" s="5"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
@@ -793,7 +798,7 @@
       <c r="D20" s="5"/>
       <c r="E20" s="14"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="14"/>
+      <c r="G20" s="22"/>
       <c r="H20" s="5"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
@@ -809,7 +814,7 @@
       <c r="D21" s="5"/>
       <c r="E21" s="14"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="14"/>
+      <c r="G21" s="22"/>
       <c r="H21" s="5"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
@@ -825,7 +830,7 @@
       <c r="D22" s="5"/>
       <c r="E22" s="14"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="14"/>
+      <c r="G22" s="22"/>
       <c r="H22" s="5"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
@@ -841,7 +846,7 @@
       <c r="D23" s="5"/>
       <c r="E23" s="14"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="14"/>
+      <c r="G23" s="22"/>
       <c r="H23" s="5"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
@@ -857,7 +862,7 @@
       <c r="D24" s="5"/>
       <c r="E24" s="14"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="14"/>
+      <c r="G24" s="22"/>
       <c r="H24" s="5"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
@@ -873,7 +878,7 @@
       <c r="D25" s="5"/>
       <c r="E25" s="14"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="14"/>
+      <c r="G25" s="22"/>
       <c r="H25" s="5"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
@@ -889,7 +894,7 @@
       <c r="D26" s="5"/>
       <c r="E26" s="14"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="14"/>
+      <c r="G26" s="22"/>
       <c r="H26" s="5"/>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
@@ -905,7 +910,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="14"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="14"/>
+      <c r="G27" s="22"/>
       <c r="H27" s="5"/>
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
@@ -921,7 +926,7 @@
       <c r="D28" s="5"/>
       <c r="E28" s="14"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="14"/>
+      <c r="G28" s="22"/>
       <c r="H28" s="5"/>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
@@ -937,7 +942,7 @@
       <c r="D29" s="5"/>
       <c r="E29" s="14"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="14"/>
+      <c r="G29" s="22"/>
       <c r="H29" s="5"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
@@ -953,7 +958,7 @@
       <c r="D30" s="5"/>
       <c r="E30" s="14"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="14"/>
+      <c r="G30" s="22"/>
       <c r="H30" s="5"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
@@ -969,7 +974,7 @@
       <c r="D31" s="5"/>
       <c r="E31" s="14"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="14"/>
+      <c r="G31" s="22"/>
       <c r="H31" s="5"/>
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
@@ -985,7 +990,7 @@
       <c r="D32" s="5"/>
       <c r="E32" s="14"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="14"/>
+      <c r="G32" s="22"/>
       <c r="H32" s="5"/>
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
@@ -1001,7 +1006,7 @@
       <c r="D33" s="5"/>
       <c r="E33" s="14"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="14"/>
+      <c r="G33" s="22"/>
       <c r="H33" s="5"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
@@ -1017,7 +1022,7 @@
       <c r="D34" s="5"/>
       <c r="E34" s="14"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="14"/>
+      <c r="G34" s="22"/>
       <c r="H34" s="5"/>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
@@ -1033,7 +1038,7 @@
       <c r="D35" s="5"/>
       <c r="E35" s="14"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="14"/>
+      <c r="G35" s="22"/>
       <c r="H35" s="5"/>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
@@ -1049,7 +1054,7 @@
       <c r="D36" s="5"/>
       <c r="E36" s="14"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="14"/>
+      <c r="G36" s="22"/>
       <c r="H36" s="5"/>
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
@@ -1065,7 +1070,7 @@
       <c r="D37" s="5"/>
       <c r="E37" s="14"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="14"/>
+      <c r="G37" s="22"/>
       <c r="H37" s="5"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
@@ -1081,7 +1086,7 @@
       <c r="D38" s="5"/>
       <c r="E38" s="14"/>
       <c r="F38" s="5"/>
-      <c r="G38" s="14"/>
+      <c r="G38" s="22"/>
       <c r="H38" s="5"/>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
@@ -1097,7 +1102,7 @@
       <c r="D39" s="5"/>
       <c r="E39" s="14"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="14"/>
+      <c r="G39" s="22"/>
       <c r="H39" s="5"/>
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
@@ -1113,7 +1118,7 @@
       <c r="D40" s="5"/>
       <c r="E40" s="14"/>
       <c r="F40" s="5"/>
-      <c r="G40" s="14"/>
+      <c r="G40" s="22"/>
       <c r="H40" s="5"/>
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
@@ -1129,7 +1134,7 @@
       <c r="D41" s="5"/>
       <c r="E41" s="14"/>
       <c r="F41" s="5"/>
-      <c r="G41" s="14"/>
+      <c r="G41" s="22"/>
       <c r="H41" s="5"/>
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
@@ -1145,7 +1150,7 @@
       <c r="D42" s="5"/>
       <c r="E42" s="14"/>
       <c r="F42" s="5"/>
-      <c r="G42" s="14"/>
+      <c r="G42" s="22"/>
       <c r="H42" s="5"/>
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
@@ -1161,7 +1166,7 @@
       <c r="D43" s="5"/>
       <c r="E43" s="14"/>
       <c r="F43" s="5"/>
-      <c r="G43" s="14"/>
+      <c r="G43" s="22"/>
       <c r="H43" s="5"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
@@ -1177,7 +1182,7 @@
       <c r="D44" s="5"/>
       <c r="E44" s="14"/>
       <c r="F44" s="5"/>
-      <c r="G44" s="14"/>
+      <c r="G44" s="22"/>
       <c r="H44" s="5"/>
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
@@ -1193,7 +1198,7 @@
       <c r="D45" s="5"/>
       <c r="E45" s="14"/>
       <c r="F45" s="5"/>
-      <c r="G45" s="14"/>
+      <c r="G45" s="22"/>
       <c r="H45" s="5"/>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
@@ -1206,7 +1211,7 @@
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="E46" s="14"/>
-      <c r="G46" s="15"/>
+      <c r="G46" s="23"/>
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
       <c r="K46" s="15"/>
@@ -1218,7 +1223,7 @@
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="E47" s="14"/>
-      <c r="G47" s="15"/>
+      <c r="G47" s="23"/>
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
       <c r="K47" s="15"/>
@@ -1230,7 +1235,7 @@
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="E48" s="14"/>
-      <c r="G48" s="15"/>
+      <c r="G48" s="23"/>
       <c r="I48" s="15"/>
       <c r="J48" s="15"/>
       <c r="K48" s="15"/>
@@ -1242,7 +1247,7 @@
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="E49" s="14"/>
-      <c r="G49" s="15"/>
+      <c r="G49" s="23"/>
       <c r="I49" s="15"/>
       <c r="J49" s="15"/>
       <c r="K49" s="15"/>
@@ -1254,7 +1259,7 @@
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="E50" s="14"/>
-      <c r="G50" s="15"/>
+      <c r="G50" s="23"/>
       <c r="I50" s="15"/>
       <c r="J50" s="15"/>
       <c r="K50" s="15"/>
@@ -1266,7 +1271,7 @@
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="E51" s="14"/>
-      <c r="G51" s="15"/>
+      <c r="G51" s="23"/>
       <c r="I51" s="15"/>
       <c r="J51" s="15"/>
       <c r="K51" s="15"/>
@@ -1278,7 +1283,7 @@
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="E52" s="14"/>
-      <c r="G52" s="15"/>
+      <c r="G52" s="23"/>
       <c r="I52" s="15"/>
       <c r="J52" s="15"/>
       <c r="K52" s="15"/>
@@ -1290,7 +1295,7 @@
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="E53" s="14"/>
-      <c r="G53" s="15"/>
+      <c r="G53" s="23"/>
       <c r="I53" s="15"/>
       <c r="J53" s="15"/>
       <c r="K53" s="15"/>
@@ -1302,7 +1307,7 @@
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="E54" s="14"/>
-      <c r="G54" s="15"/>
+      <c r="G54" s="23"/>
       <c r="I54" s="15"/>
       <c r="J54" s="15"/>
       <c r="K54" s="15"/>
@@ -1314,7 +1319,7 @@
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="E55" s="14"/>
-      <c r="G55" s="15"/>
+      <c r="G55" s="23"/>
       <c r="I55" s="15"/>
       <c r="J55" s="15"/>
       <c r="K55" s="15"/>
@@ -1326,7 +1331,7 @@
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="E56" s="14"/>
-      <c r="G56" s="15"/>
+      <c r="G56" s="23"/>
       <c r="I56" s="15"/>
       <c r="J56" s="15"/>
       <c r="K56" s="15"/>
@@ -1338,7 +1343,7 @@
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="E57" s="14"/>
-      <c r="G57" s="15"/>
+      <c r="G57" s="23"/>
       <c r="I57" s="15"/>
       <c r="J57" s="15"/>
       <c r="K57" s="15"/>
@@ -1350,7 +1355,7 @@
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="E58" s="14"/>
-      <c r="G58" s="15"/>
+      <c r="G58" s="23"/>
       <c r="I58" s="15"/>
       <c r="J58" s="15"/>
       <c r="K58" s="15"/>
@@ -1362,7 +1367,7 @@
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="E59" s="14"/>
-      <c r="G59" s="15"/>
+      <c r="G59" s="23"/>
       <c r="I59" s="15"/>
       <c r="J59" s="15"/>
       <c r="K59" s="15"/>
@@ -1374,7 +1379,7 @@
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="E60" s="14"/>
-      <c r="G60" s="15"/>
+      <c r="G60" s="23"/>
       <c r="I60" s="15"/>
       <c r="J60" s="15"/>
       <c r="K60" s="15"/>
@@ -1386,7 +1391,7 @@
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="E61" s="14"/>
-      <c r="G61" s="15"/>
+      <c r="G61" s="23"/>
       <c r="I61" s="15"/>
       <c r="J61" s="15"/>
       <c r="K61" s="15"/>
@@ -1398,7 +1403,7 @@
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="E62" s="14"/>
-      <c r="G62" s="15"/>
+      <c r="G62" s="23"/>
       <c r="I62" s="15"/>
       <c r="J62" s="15"/>
       <c r="K62" s="15"/>
@@ -1410,7 +1415,7 @@
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="E63" s="14"/>
-      <c r="G63" s="15"/>
+      <c r="G63" s="23"/>
       <c r="I63" s="15"/>
       <c r="J63" s="15"/>
       <c r="K63" s="15"/>
@@ -1422,7 +1427,7 @@
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="E64" s="14"/>
-      <c r="G64" s="15"/>
+      <c r="G64" s="23"/>
       <c r="I64" s="15"/>
       <c r="J64" s="15"/>
       <c r="K64" s="15"/>
@@ -1433,7 +1438,7 @@
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="E65" s="14"/>
-      <c r="G65" s="15"/>
+      <c r="G65" s="23"/>
       <c r="I65" s="15"/>
       <c r="J65" s="15"/>
       <c r="K65" s="15"/>
@@ -1444,7 +1449,7 @@
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="E66" s="14"/>
-      <c r="G66" s="15"/>
+      <c r="G66" s="23"/>
       <c r="I66" s="15"/>
       <c r="J66" s="15"/>
       <c r="K66" s="15"/>
@@ -1455,7 +1460,7 @@
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="E67" s="14"/>
-      <c r="G67" s="15"/>
+      <c r="G67" s="23"/>
       <c r="I67" s="15"/>
       <c r="J67" s="15"/>
       <c r="K67" s="15"/>
@@ -1466,7 +1471,7 @@
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="E68" s="14"/>
-      <c r="G68" s="15"/>
+      <c r="G68" s="23"/>
       <c r="I68" s="15"/>
       <c r="J68" s="15"/>
       <c r="K68" s="15"/>
@@ -1477,7 +1482,7 @@
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="E69" s="14"/>
-      <c r="G69" s="15"/>
+      <c r="G69" s="23"/>
       <c r="I69" s="15"/>
       <c r="J69" s="15"/>
       <c r="K69" s="15"/>
@@ -1488,7 +1493,7 @@
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="E70" s="14"/>
-      <c r="G70" s="15"/>
+      <c r="G70" s="23"/>
       <c r="I70" s="15"/>
       <c r="J70" s="15"/>
       <c r="K70" s="15"/>
@@ -1499,7 +1504,7 @@
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="E71" s="14"/>
-      <c r="G71" s="15"/>
+      <c r="G71" s="23"/>
       <c r="I71" s="15"/>
       <c r="J71" s="15"/>
       <c r="K71" s="15"/>
@@ -1510,7 +1515,7 @@
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="E72" s="14"/>
-      <c r="G72" s="15"/>
+      <c r="G72" s="23"/>
       <c r="I72" s="15"/>
       <c r="J72" s="15"/>
       <c r="K72" s="15"/>
@@ -1521,7 +1526,7 @@
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="E73" s="14"/>
-      <c r="G73" s="15"/>
+      <c r="G73" s="23"/>
       <c r="I73" s="15"/>
       <c r="J73" s="15"/>
       <c r="K73" s="15"/>
@@ -1532,7 +1537,7 @@
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="E74" s="14"/>
-      <c r="G74" s="15"/>
+      <c r="G74" s="23"/>
       <c r="I74" s="15"/>
       <c r="J74" s="15"/>
       <c r="K74" s="15"/>
@@ -1543,7 +1548,7 @@
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="E75" s="14"/>
-      <c r="G75" s="15"/>
+      <c r="G75" s="23"/>
       <c r="I75" s="15"/>
       <c r="J75" s="15"/>
       <c r="K75" s="15"/>
@@ -1554,7 +1559,7 @@
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="E76" s="14"/>
-      <c r="G76" s="15"/>
+      <c r="G76" s="23"/>
       <c r="I76" s="15"/>
       <c r="J76" s="15"/>
       <c r="K76" s="15"/>
@@ -1565,7 +1570,7 @@
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="E77" s="14"/>
-      <c r="G77" s="15"/>
+      <c r="G77" s="23"/>
       <c r="I77" s="15"/>
       <c r="J77" s="15"/>
       <c r="K77" s="15"/>
@@ -1576,7 +1581,7 @@
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="E78" s="14"/>
-      <c r="G78" s="15"/>
+      <c r="G78" s="23"/>
       <c r="I78" s="15"/>
       <c r="J78" s="15"/>
       <c r="K78" s="15"/>
@@ -1587,7 +1592,7 @@
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="E79" s="14"/>
-      <c r="G79" s="15"/>
+      <c r="G79" s="23"/>
       <c r="I79" s="15"/>
       <c r="J79" s="15"/>
       <c r="K79" s="15"/>
@@ -1598,7 +1603,7 @@
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="E80" s="14"/>
-      <c r="G80" s="15"/>
+      <c r="G80" s="23"/>
       <c r="I80" s="15"/>
       <c r="J80" s="15"/>
       <c r="K80" s="15"/>
@@ -1609,7 +1614,7 @@
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="E81" s="14"/>
-      <c r="G81" s="15"/>
+      <c r="G81" s="23"/>
       <c r="I81" s="15"/>
       <c r="J81" s="15"/>
       <c r="K81" s="15"/>
@@ -1620,7 +1625,7 @@
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="E82" s="14"/>
-      <c r="G82" s="15"/>
+      <c r="G82" s="23"/>
       <c r="I82" s="15"/>
       <c r="J82" s="15"/>
       <c r="K82" s="15"/>
@@ -1631,7 +1636,7 @@
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="E83" s="14"/>
-      <c r="G83" s="15"/>
+      <c r="G83" s="23"/>
       <c r="I83" s="15"/>
       <c r="J83" s="15"/>
       <c r="K83" s="15"/>
@@ -1642,7 +1647,7 @@
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="E84" s="14"/>
-      <c r="G84" s="15"/>
+      <c r="G84" s="23"/>
       <c r="I84" s="15"/>
       <c r="J84" s="15"/>
       <c r="K84" s="15"/>
@@ -1653,7 +1658,7 @@
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="E85" s="14"/>
-      <c r="G85" s="15"/>
+      <c r="G85" s="23"/>
       <c r="I85" s="15"/>
       <c r="J85" s="15"/>
       <c r="K85" s="15"/>
@@ -1664,7 +1669,7 @@
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="E86" s="14"/>
-      <c r="G86" s="15"/>
+      <c r="G86" s="23"/>
       <c r="I86" s="15"/>
       <c r="J86" s="15"/>
       <c r="K86" s="15"/>
@@ -1675,7 +1680,7 @@
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="E87" s="14"/>
-      <c r="G87" s="15"/>
+      <c r="G87" s="23"/>
       <c r="I87" s="15"/>
       <c r="J87" s="15"/>
       <c r="K87" s="15"/>
@@ -1686,7 +1691,7 @@
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="E88" s="14"/>
-      <c r="G88" s="15"/>
+      <c r="G88" s="23"/>
       <c r="I88" s="15"/>
       <c r="J88" s="15"/>
       <c r="K88" s="15"/>
@@ -1697,7 +1702,7 @@
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="E89" s="14"/>
-      <c r="G89" s="15"/>
+      <c r="G89" s="23"/>
       <c r="I89" s="15"/>
       <c r="J89" s="15"/>
       <c r="K89" s="15"/>
@@ -1708,7 +1713,7 @@
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="E90" s="14"/>
-      <c r="G90" s="15"/>
+      <c r="G90" s="23"/>
       <c r="I90" s="15"/>
       <c r="J90" s="15"/>
       <c r="K90" s="15"/>
@@ -1719,7 +1724,7 @@
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="E91" s="14"/>
-      <c r="G91" s="15"/>
+      <c r="G91" s="23"/>
       <c r="I91" s="15"/>
       <c r="J91" s="15"/>
       <c r="K91" s="15"/>
@@ -1730,7 +1735,7 @@
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="E92" s="14"/>
-      <c r="G92" s="15"/>
+      <c r="G92" s="23"/>
       <c r="I92" s="15"/>
       <c r="J92" s="15"/>
       <c r="K92" s="15"/>
@@ -1741,7 +1746,7 @@
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="E93" s="14"/>
-      <c r="G93" s="15"/>
+      <c r="G93" s="23"/>
       <c r="I93" s="15"/>
       <c r="J93" s="15"/>
       <c r="K93" s="15"/>
@@ -1752,7 +1757,7 @@
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="E94" s="14"/>
-      <c r="G94" s="15"/>
+      <c r="G94" s="23"/>
       <c r="I94" s="15"/>
       <c r="J94" s="15"/>
       <c r="K94" s="15"/>
@@ -1763,7 +1768,7 @@
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="E95" s="14"/>
-      <c r="G95" s="15"/>
+      <c r="G95" s="23"/>
       <c r="I95" s="15"/>
       <c r="J95" s="15"/>
       <c r="K95" s="15"/>
@@ -1774,7 +1779,7 @@
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="E96" s="14"/>
-      <c r="G96" s="15"/>
+      <c r="G96" s="23"/>
       <c r="I96" s="15"/>
       <c r="J96" s="15"/>
       <c r="K96" s="15"/>
@@ -1785,7 +1790,7 @@
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="E97" s="14"/>
-      <c r="G97" s="15"/>
+      <c r="G97" s="23"/>
       <c r="I97" s="15"/>
       <c r="J97" s="15"/>
       <c r="K97" s="15"/>
@@ -1796,7 +1801,7 @@
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="E98" s="14"/>
-      <c r="G98" s="15"/>
+      <c r="G98" s="23"/>
       <c r="I98" s="15"/>
       <c r="J98" s="15"/>
       <c r="K98" s="15"/>
@@ -1807,7 +1812,7 @@
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="E99" s="14"/>
-      <c r="G99" s="15"/>
+      <c r="G99" s="23"/>
       <c r="I99" s="15"/>
       <c r="J99" s="15"/>
       <c r="K99" s="15"/>
@@ -1818,7 +1823,7 @@
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="E100" s="14"/>
-      <c r="G100" s="15"/>
+      <c r="G100" s="23"/>
       <c r="I100" s="15"/>
       <c r="J100" s="15"/>
       <c r="K100" s="15"/>
@@ -1829,7 +1834,7 @@
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="E101" s="14"/>
-      <c r="G101" s="15"/>
+      <c r="G101" s="23"/>
       <c r="I101" s="15"/>
       <c r="J101" s="15"/>
       <c r="K101" s="15"/>
@@ -1840,7 +1845,7 @@
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="E102" s="14"/>
-      <c r="G102" s="15"/>
+      <c r="G102" s="23"/>
       <c r="I102" s="15"/>
       <c r="J102" s="15"/>
       <c r="K102" s="15"/>
@@ -1851,7 +1856,7 @@
     <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="E103" s="14"/>
-      <c r="G103" s="15"/>
+      <c r="G103" s="23"/>
       <c r="I103" s="15"/>
       <c r="J103" s="15"/>
       <c r="K103" s="15"/>
@@ -1862,7 +1867,7 @@
     <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="E104" s="14"/>
-      <c r="G104" s="15"/>
+      <c r="G104" s="23"/>
       <c r="I104" s="15"/>
       <c r="J104" s="15"/>
       <c r="K104" s="15"/>
@@ -1873,7 +1878,7 @@
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="E105" s="14"/>
-      <c r="G105" s="15"/>
+      <c r="G105" s="23"/>
       <c r="I105" s="15"/>
       <c r="J105" s="15"/>
       <c r="K105" s="15"/>
@@ -1884,7 +1889,7 @@
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="E106" s="14"/>
-      <c r="G106" s="15"/>
+      <c r="G106" s="23"/>
       <c r="I106" s="15"/>
       <c r="J106" s="15"/>
       <c r="K106" s="15"/>
@@ -1895,7 +1900,7 @@
     <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="E107" s="14"/>
-      <c r="G107" s="15"/>
+      <c r="G107" s="23"/>
       <c r="I107" s="15"/>
       <c r="J107" s="15"/>
       <c r="K107" s="15"/>
@@ -1905,7 +1910,7 @@
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E108" s="14"/>
-      <c r="G108" s="15"/>
+      <c r="G108" s="23"/>
       <c r="I108" s="15"/>
       <c r="J108" s="15"/>
       <c r="K108" s="15"/>
@@ -1915,7 +1920,7 @@
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E109" s="14"/>
-      <c r="G109" s="15"/>
+      <c r="G109" s="23"/>
       <c r="I109" s="15"/>
       <c r="J109" s="15"/>
       <c r="K109" s="15"/>
@@ -1925,7 +1930,7 @@
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E110" s="14"/>
-      <c r="G110" s="15"/>
+      <c r="G110" s="23"/>
       <c r="I110" s="15"/>
       <c r="J110" s="15"/>
       <c r="K110" s="15"/>
@@ -1935,7 +1940,7 @@
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E111" s="14"/>
-      <c r="G111" s="15"/>
+      <c r="G111" s="23"/>
       <c r="I111" s="15"/>
       <c r="J111" s="15"/>
       <c r="K111" s="15"/>
@@ -1945,7 +1950,7 @@
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E112" s="14"/>
-      <c r="G112" s="15"/>
+      <c r="G112" s="23"/>
       <c r="I112" s="15"/>
       <c r="J112" s="15"/>
       <c r="K112" s="15"/>
@@ -1955,7 +1960,7 @@
     </row>
     <row r="113" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E113" s="14"/>
-      <c r="G113" s="15"/>
+      <c r="G113" s="23"/>
       <c r="I113" s="15"/>
       <c r="J113" s="15"/>
       <c r="K113" s="15"/>
@@ -1965,7 +1970,7 @@
     </row>
     <row r="114" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E114" s="14"/>
-      <c r="G114" s="15"/>
+      <c r="G114" s="23"/>
       <c r="I114" s="15"/>
       <c r="J114" s="15"/>
       <c r="K114" s="15"/>
@@ -1975,7 +1980,7 @@
     </row>
     <row r="115" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E115" s="14"/>
-      <c r="G115" s="15"/>
+      <c r="G115" s="23"/>
       <c r="I115" s="15"/>
       <c r="J115" s="15"/>
       <c r="K115" s="15"/>
@@ -1985,6 +1990,7 @@
     </row>
     <row r="116" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E116" s="14"/>
+      <c r="G116" s="23"/>
       <c r="I116" s="15"/>
       <c r="J116" s="15"/>
       <c r="K116" s="15"/>
@@ -1994,6 +2000,7 @@
     </row>
     <row r="117" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E117" s="14"/>
+      <c r="G117" s="23"/>
       <c r="I117" s="15"/>
       <c r="J117" s="15"/>
       <c r="K117" s="15"/>
@@ -2003,6 +2010,7 @@
     </row>
     <row r="118" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E118" s="14"/>
+      <c r="G118" s="23"/>
       <c r="I118" s="15"/>
       <c r="J118" s="15"/>
       <c r="K118" s="15"/>
@@ -2012,6 +2020,7 @@
     </row>
     <row r="119" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E119" s="14"/>
+      <c r="G119" s="23"/>
       <c r="I119" s="15"/>
       <c r="J119" s="15"/>
       <c r="K119" s="15"/>
@@ -2021,6 +2030,7 @@
     </row>
     <row r="120" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E120" s="14"/>
+      <c r="G120" s="23"/>
       <c r="I120" s="15"/>
       <c r="J120" s="15"/>
       <c r="K120" s="15"/>
@@ -2030,6 +2040,7 @@
     </row>
     <row r="121" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E121" s="14"/>
+      <c r="G121" s="23"/>
       <c r="I121" s="15"/>
       <c r="J121" s="15"/>
       <c r="K121" s="15"/>
@@ -2039,6 +2050,7 @@
     </row>
     <row r="122" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E122" s="14"/>
+      <c r="G122" s="23"/>
       <c r="I122" s="15"/>
       <c r="J122" s="15"/>
       <c r="K122" s="15"/>
@@ -2048,6 +2060,7 @@
     </row>
     <row r="123" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E123" s="14"/>
+      <c r="G123" s="23"/>
       <c r="I123" s="15"/>
       <c r="J123" s="15"/>
       <c r="K123" s="15"/>
@@ -2057,6 +2070,7 @@
     </row>
     <row r="124" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E124" s="14"/>
+      <c r="G124" s="23"/>
       <c r="I124" s="15"/>
       <c r="J124" s="15"/>
       <c r="K124" s="15"/>
@@ -2066,6 +2080,7 @@
     </row>
     <row r="125" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E125" s="14"/>
+      <c r="G125" s="23"/>
       <c r="I125" s="15"/>
       <c r="J125" s="15"/>
       <c r="K125" s="15"/>
@@ -2075,6 +2090,7 @@
     </row>
     <row r="126" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E126" s="14"/>
+      <c r="G126" s="23"/>
       <c r="I126" s="15"/>
       <c r="J126" s="15"/>
       <c r="K126" s="15"/>
@@ -2084,6 +2100,7 @@
     </row>
     <row r="127" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E127" s="14"/>
+      <c r="G127" s="23"/>
       <c r="I127" s="15"/>
       <c r="J127" s="15"/>
       <c r="K127" s="15"/>
@@ -2093,930 +2110,1564 @@
     </row>
     <row r="128" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E128" s="14"/>
+      <c r="G128" s="23"/>
       <c r="N128" s="14"/>
     </row>
     <row r="129" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E129" s="14"/>
+      <c r="G129" s="23"/>
       <c r="N129" s="14"/>
     </row>
     <row r="130" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E130" s="14"/>
+      <c r="G130" s="23"/>
       <c r="N130" s="14"/>
     </row>
     <row r="131" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E131" s="14"/>
+      <c r="G131" s="23"/>
       <c r="N131" s="14"/>
     </row>
     <row r="132" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E132" s="14"/>
+      <c r="G132" s="23"/>
       <c r="N132" s="14"/>
     </row>
     <row r="133" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E133" s="14"/>
+      <c r="G133" s="23"/>
       <c r="N133" s="14"/>
     </row>
     <row r="134" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E134" s="14"/>
+      <c r="G134" s="23"/>
       <c r="N134" s="14"/>
     </row>
     <row r="135" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E135" s="14"/>
+      <c r="G135" s="23"/>
       <c r="N135" s="14"/>
     </row>
     <row r="136" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E136" s="14"/>
+      <c r="G136" s="23"/>
       <c r="N136" s="14"/>
     </row>
     <row r="137" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E137" s="14"/>
+      <c r="G137" s="23"/>
       <c r="N137" s="14"/>
     </row>
     <row r="138" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E138" s="14"/>
+      <c r="G138" s="23"/>
       <c r="N138" s="14"/>
     </row>
     <row r="139" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E139" s="14"/>
+      <c r="G139" s="23"/>
       <c r="N139" s="14"/>
     </row>
     <row r="140" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E140" s="14"/>
+      <c r="G140" s="23"/>
       <c r="N140" s="14"/>
     </row>
     <row r="141" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E141" s="14"/>
+      <c r="G141" s="23"/>
       <c r="N141" s="14"/>
     </row>
     <row r="142" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E142" s="14"/>
+      <c r="G142" s="23"/>
       <c r="N142" s="14"/>
     </row>
     <row r="143" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E143" s="14"/>
+      <c r="G143" s="23"/>
       <c r="N143" s="14"/>
     </row>
     <row r="144" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E144" s="14"/>
+      <c r="G144" s="23"/>
       <c r="N144" s="14"/>
     </row>
     <row r="145" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E145" s="14"/>
+      <c r="G145" s="23"/>
       <c r="N145" s="14"/>
     </row>
     <row r="146" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E146" s="14"/>
+      <c r="G146" s="23"/>
       <c r="N146" s="14"/>
     </row>
     <row r="147" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E147" s="14"/>
+      <c r="G147" s="23"/>
       <c r="N147" s="14"/>
     </row>
     <row r="148" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E148" s="14"/>
+      <c r="G148" s="23"/>
       <c r="N148" s="14"/>
     </row>
     <row r="149" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E149" s="14"/>
+      <c r="G149" s="23"/>
       <c r="N149" s="14"/>
     </row>
     <row r="150" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E150" s="14"/>
+      <c r="G150" s="23"/>
       <c r="N150" s="14"/>
     </row>
     <row r="151" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E151" s="14"/>
+      <c r="G151" s="23"/>
       <c r="N151" s="14"/>
     </row>
     <row r="152" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E152" s="14"/>
+      <c r="G152" s="23"/>
       <c r="N152" s="14"/>
     </row>
     <row r="153" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E153" s="14"/>
+      <c r="G153" s="23"/>
       <c r="N153" s="14"/>
     </row>
     <row r="154" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E154" s="14"/>
+      <c r="G154" s="23"/>
       <c r="N154" s="14"/>
     </row>
     <row r="155" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E155" s="14"/>
+      <c r="G155" s="23"/>
       <c r="N155" s="14"/>
     </row>
     <row r="156" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E156" s="14"/>
+      <c r="G156" s="23"/>
       <c r="N156" s="14"/>
     </row>
     <row r="157" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E157" s="14"/>
+      <c r="G157" s="23"/>
       <c r="N157" s="14"/>
     </row>
     <row r="158" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E158" s="14"/>
+      <c r="G158" s="23"/>
       <c r="N158" s="14"/>
     </row>
     <row r="159" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E159" s="14"/>
+      <c r="G159" s="23"/>
       <c r="N159" s="14"/>
     </row>
     <row r="160" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E160" s="14"/>
+      <c r="G160" s="23"/>
       <c r="N160" s="14"/>
     </row>
     <row r="161" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E161" s="14"/>
+      <c r="G161" s="23"/>
       <c r="N161" s="14"/>
     </row>
     <row r="162" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E162" s="14"/>
+      <c r="G162" s="23"/>
       <c r="N162" s="14"/>
     </row>
     <row r="163" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E163" s="14"/>
+      <c r="G163" s="23"/>
       <c r="N163" s="14"/>
     </row>
     <row r="164" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E164" s="14"/>
+      <c r="G164" s="23"/>
       <c r="N164" s="14"/>
     </row>
     <row r="165" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E165" s="14"/>
+      <c r="G165" s="23"/>
       <c r="N165" s="14"/>
     </row>
     <row r="166" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E166" s="14"/>
+      <c r="G166" s="23"/>
       <c r="N166" s="14"/>
     </row>
     <row r="167" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E167" s="14"/>
+      <c r="G167" s="23"/>
       <c r="N167" s="14"/>
     </row>
     <row r="168" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E168" s="14"/>
+      <c r="G168" s="23"/>
       <c r="N168" s="14"/>
     </row>
     <row r="169" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E169" s="14"/>
+      <c r="G169" s="23"/>
       <c r="N169" s="14"/>
     </row>
     <row r="170" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E170" s="14"/>
+      <c r="G170" s="23"/>
       <c r="N170" s="14"/>
     </row>
     <row r="171" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E171" s="14"/>
+      <c r="G171" s="23"/>
       <c r="N171" s="14"/>
     </row>
     <row r="172" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E172" s="14"/>
+      <c r="G172" s="23"/>
       <c r="N172" s="14"/>
     </row>
     <row r="173" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E173" s="14"/>
+      <c r="G173" s="23"/>
       <c r="N173" s="14"/>
     </row>
     <row r="174" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E174" s="14"/>
+      <c r="G174" s="23"/>
       <c r="N174" s="14"/>
     </row>
     <row r="175" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E175" s="14"/>
+      <c r="G175" s="23"/>
       <c r="N175" s="14"/>
     </row>
     <row r="176" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E176" s="14"/>
+      <c r="G176" s="23"/>
       <c r="N176" s="14"/>
     </row>
     <row r="177" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E177" s="14"/>
+      <c r="G177" s="23"/>
       <c r="N177" s="14"/>
     </row>
     <row r="178" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E178" s="14"/>
+      <c r="G178" s="23"/>
       <c r="N178" s="14"/>
     </row>
     <row r="179" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E179" s="14"/>
+      <c r="G179" s="23"/>
       <c r="N179" s="14"/>
     </row>
     <row r="180" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E180" s="14"/>
+      <c r="G180" s="23"/>
       <c r="N180" s="14"/>
     </row>
     <row r="181" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E181" s="14"/>
+      <c r="G181" s="23"/>
       <c r="N181" s="14"/>
     </row>
     <row r="182" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E182" s="14"/>
+      <c r="G182" s="23"/>
       <c r="N182" s="14"/>
     </row>
     <row r="183" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E183" s="14"/>
+      <c r="G183" s="23"/>
       <c r="N183" s="14"/>
     </row>
     <row r="184" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E184" s="14"/>
+      <c r="G184" s="23"/>
       <c r="N184" s="14"/>
     </row>
     <row r="185" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E185" s="14"/>
+      <c r="G185" s="23"/>
       <c r="N185" s="14"/>
     </row>
     <row r="186" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E186" s="14"/>
+      <c r="G186" s="23"/>
       <c r="N186" s="14"/>
     </row>
     <row r="187" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E187" s="14"/>
+      <c r="G187" s="23"/>
       <c r="N187" s="14"/>
     </row>
     <row r="188" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E188" s="14"/>
+      <c r="G188" s="23"/>
       <c r="N188" s="14"/>
     </row>
     <row r="189" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E189" s="14"/>
+      <c r="G189" s="23"/>
       <c r="N189" s="14"/>
     </row>
     <row r="190" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E190" s="14"/>
+      <c r="G190" s="23"/>
       <c r="N190" s="14"/>
     </row>
     <row r="191" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E191" s="14"/>
+      <c r="G191" s="23"/>
       <c r="N191" s="14"/>
     </row>
     <row r="192" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E192" s="14"/>
+      <c r="G192" s="23"/>
       <c r="N192" s="14"/>
     </row>
     <row r="193" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E193" s="14"/>
+      <c r="G193" s="23"/>
       <c r="N193" s="14"/>
     </row>
     <row r="194" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E194" s="14"/>
+      <c r="G194" s="23"/>
       <c r="N194" s="14"/>
     </row>
     <row r="195" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E195" s="14"/>
+      <c r="G195" s="23"/>
       <c r="N195" s="14"/>
     </row>
     <row r="196" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E196" s="14"/>
+      <c r="G196" s="23"/>
       <c r="N196" s="14"/>
     </row>
     <row r="197" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E197" s="14"/>
+      <c r="G197" s="23"/>
       <c r="N197" s="14"/>
     </row>
     <row r="198" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E198" s="14"/>
+      <c r="G198" s="23"/>
       <c r="N198" s="14"/>
     </row>
     <row r="199" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E199" s="14"/>
+      <c r="G199" s="23"/>
       <c r="N199" s="14"/>
     </row>
     <row r="200" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E200" s="14"/>
+      <c r="G200" s="23"/>
       <c r="N200" s="14"/>
     </row>
     <row r="201" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E201" s="14"/>
+      <c r="G201" s="23"/>
       <c r="N201" s="14"/>
     </row>
     <row r="202" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E202" s="14"/>
+      <c r="G202" s="23"/>
       <c r="N202" s="14"/>
     </row>
     <row r="203" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E203" s="14"/>
+      <c r="G203" s="23"/>
       <c r="N203" s="14"/>
     </row>
     <row r="204" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E204" s="14"/>
+      <c r="G204" s="23"/>
       <c r="N204" s="14"/>
     </row>
     <row r="205" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E205" s="14"/>
+      <c r="G205" s="23"/>
       <c r="N205" s="14"/>
     </row>
     <row r="206" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E206" s="14"/>
+      <c r="G206" s="23"/>
       <c r="N206" s="14"/>
     </row>
     <row r="207" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E207" s="14"/>
+      <c r="G207" s="23"/>
       <c r="N207" s="14"/>
     </row>
     <row r="208" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E208" s="14"/>
+      <c r="G208" s="23"/>
       <c r="N208" s="14"/>
     </row>
     <row r="209" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E209" s="14"/>
+      <c r="G209" s="23"/>
       <c r="N209" s="14"/>
     </row>
     <row r="210" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E210" s="14"/>
+      <c r="G210" s="23"/>
       <c r="N210" s="14"/>
     </row>
     <row r="211" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E211" s="14"/>
+      <c r="G211" s="23"/>
       <c r="N211" s="14"/>
     </row>
     <row r="212" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E212" s="14"/>
+      <c r="G212" s="23"/>
       <c r="N212" s="14"/>
     </row>
     <row r="213" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E213" s="14"/>
+      <c r="G213" s="23"/>
       <c r="N213" s="14"/>
     </row>
     <row r="214" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E214" s="14"/>
+      <c r="G214" s="23"/>
       <c r="N214" s="14"/>
     </row>
     <row r="215" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E215" s="14"/>
+      <c r="G215" s="23"/>
       <c r="N215" s="14"/>
     </row>
     <row r="216" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E216" s="14"/>
+      <c r="G216" s="23"/>
       <c r="N216" s="14"/>
     </row>
     <row r="217" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E217" s="14"/>
+      <c r="G217" s="23"/>
       <c r="N217" s="14"/>
     </row>
     <row r="218" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E218" s="14"/>
+      <c r="G218" s="23"/>
       <c r="N218" s="14"/>
     </row>
     <row r="219" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E219" s="14"/>
+      <c r="G219" s="23"/>
       <c r="N219" s="14"/>
     </row>
     <row r="220" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E220" s="14"/>
+      <c r="G220" s="23"/>
       <c r="N220" s="14"/>
     </row>
     <row r="221" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E221" s="14"/>
+      <c r="G221" s="23"/>
       <c r="N221" s="14"/>
     </row>
     <row r="222" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E222" s="14"/>
+      <c r="G222" s="23"/>
       <c r="N222" s="14"/>
     </row>
     <row r="223" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E223" s="14"/>
+      <c r="G223" s="23"/>
       <c r="N223" s="14"/>
     </row>
     <row r="224" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E224" s="14"/>
+      <c r="G224" s="23"/>
       <c r="N224" s="14"/>
     </row>
     <row r="225" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E225" s="14"/>
+      <c r="G225" s="23"/>
       <c r="N225" s="14"/>
     </row>
     <row r="226" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E226" s="14"/>
+      <c r="G226" s="23"/>
       <c r="N226" s="14"/>
     </row>
     <row r="227" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E227" s="14"/>
+      <c r="G227" s="23"/>
       <c r="N227" s="14"/>
     </row>
     <row r="228" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E228" s="14"/>
+      <c r="G228" s="23"/>
       <c r="N228" s="14"/>
     </row>
     <row r="229" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E229" s="14"/>
+      <c r="G229" s="23"/>
       <c r="N229" s="14"/>
     </row>
     <row r="230" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E230" s="14"/>
+      <c r="G230" s="23"/>
       <c r="N230" s="14"/>
     </row>
     <row r="231" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E231" s="14"/>
+      <c r="G231" s="23"/>
       <c r="N231" s="14"/>
     </row>
     <row r="232" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E232" s="14"/>
+      <c r="G232" s="23"/>
       <c r="N232" s="14"/>
     </row>
     <row r="233" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E233" s="14"/>
+      <c r="G233" s="23"/>
       <c r="N233" s="14"/>
     </row>
     <row r="234" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E234" s="14"/>
+      <c r="G234" s="23"/>
       <c r="N234" s="14"/>
     </row>
     <row r="235" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E235" s="14"/>
+      <c r="G235" s="23"/>
       <c r="N235" s="14"/>
     </row>
     <row r="236" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E236" s="14"/>
+      <c r="G236" s="23"/>
       <c r="N236" s="14"/>
     </row>
     <row r="237" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E237" s="14"/>
+      <c r="G237" s="23"/>
       <c r="N237" s="14"/>
     </row>
     <row r="238" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E238" s="14"/>
+      <c r="G238" s="23"/>
       <c r="N238" s="14"/>
     </row>
     <row r="239" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E239" s="14"/>
+      <c r="G239" s="23"/>
       <c r="N239" s="14"/>
     </row>
     <row r="240" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E240" s="14"/>
+      <c r="G240" s="23"/>
       <c r="N240" s="14"/>
     </row>
     <row r="241" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E241" s="14"/>
+      <c r="G241" s="23"/>
       <c r="N241" s="14"/>
     </row>
     <row r="242" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E242" s="14"/>
+      <c r="G242" s="23"/>
       <c r="N242" s="14"/>
     </row>
     <row r="243" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E243" s="14"/>
+      <c r="G243" s="23"/>
       <c r="N243" s="14"/>
     </row>
     <row r="244" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E244" s="14"/>
+      <c r="G244" s="23"/>
       <c r="N244" s="14"/>
     </row>
     <row r="245" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E245" s="14"/>
+      <c r="G245" s="23"/>
       <c r="N245" s="14"/>
     </row>
     <row r="246" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E246" s="14"/>
+      <c r="G246" s="23"/>
       <c r="N246" s="14"/>
     </row>
     <row r="247" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E247" s="14"/>
+      <c r="G247" s="23"/>
       <c r="N247" s="14"/>
     </row>
     <row r="248" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E248" s="14"/>
+      <c r="G248" s="23"/>
       <c r="N248" s="14"/>
     </row>
     <row r="249" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E249" s="14"/>
+      <c r="G249" s="23"/>
       <c r="N249" s="14"/>
     </row>
     <row r="250" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E250" s="14"/>
+      <c r="G250" s="23"/>
       <c r="N250" s="14"/>
     </row>
     <row r="251" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E251" s="14"/>
+      <c r="G251" s="23"/>
       <c r="N251" s="14"/>
     </row>
     <row r="252" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E252" s="14"/>
+      <c r="G252" s="23"/>
       <c r="N252" s="14"/>
     </row>
     <row r="253" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E253" s="14"/>
+      <c r="G253" s="23"/>
       <c r="N253" s="14"/>
     </row>
     <row r="254" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E254" s="14"/>
+      <c r="G254" s="23"/>
       <c r="N254" s="14"/>
     </row>
     <row r="255" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E255" s="14"/>
+      <c r="G255" s="23"/>
       <c r="N255" s="14"/>
     </row>
     <row r="256" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E256" s="14"/>
+      <c r="G256" s="23"/>
       <c r="N256" s="14"/>
     </row>
     <row r="257" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E257" s="14"/>
+      <c r="G257" s="23"/>
       <c r="N257" s="14"/>
     </row>
     <row r="258" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E258" s="14"/>
+      <c r="G258" s="23"/>
       <c r="N258" s="14"/>
     </row>
     <row r="259" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E259" s="14"/>
+      <c r="G259" s="23"/>
       <c r="N259" s="14"/>
     </row>
     <row r="260" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E260" s="14"/>
+      <c r="G260" s="23"/>
       <c r="N260" s="14"/>
     </row>
     <row r="261" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E261" s="14"/>
+      <c r="G261" s="23"/>
       <c r="N261" s="14"/>
     </row>
     <row r="262" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E262" s="14"/>
+      <c r="G262" s="23"/>
       <c r="N262" s="14"/>
     </row>
     <row r="263" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E263" s="14"/>
+      <c r="G263" s="23"/>
       <c r="N263" s="14"/>
     </row>
     <row r="264" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E264" s="14"/>
+      <c r="G264" s="23"/>
       <c r="N264" s="14"/>
     </row>
     <row r="265" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E265" s="14"/>
+      <c r="G265" s="23"/>
       <c r="N265" s="14"/>
     </row>
     <row r="266" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E266" s="14"/>
+      <c r="G266" s="23"/>
       <c r="N266" s="14"/>
     </row>
     <row r="267" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E267" s="14"/>
+      <c r="G267" s="23"/>
       <c r="N267" s="14"/>
     </row>
     <row r="268" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E268" s="14"/>
+      <c r="G268" s="23"/>
       <c r="N268" s="14"/>
     </row>
     <row r="269" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E269" s="14"/>
+      <c r="G269" s="23"/>
       <c r="N269" s="14"/>
     </row>
     <row r="270" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E270" s="14"/>
+      <c r="G270" s="23"/>
       <c r="N270" s="14"/>
     </row>
     <row r="271" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E271" s="14"/>
+      <c r="G271" s="23"/>
       <c r="N271" s="14"/>
     </row>
     <row r="272" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E272" s="14"/>
+      <c r="G272" s="23"/>
       <c r="N272" s="14"/>
     </row>
     <row r="273" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E273" s="14"/>
+      <c r="G273" s="23"/>
       <c r="N273" s="14"/>
     </row>
     <row r="274" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E274" s="14"/>
+      <c r="G274" s="23"/>
       <c r="N274" s="14"/>
     </row>
     <row r="275" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E275" s="14"/>
+      <c r="G275" s="23"/>
       <c r="N275" s="14"/>
     </row>
     <row r="276" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E276" s="14"/>
+      <c r="G276" s="23"/>
       <c r="N276" s="14"/>
     </row>
     <row r="277" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E277" s="14"/>
+      <c r="G277" s="23"/>
       <c r="N277" s="14"/>
     </row>
     <row r="278" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E278" s="14"/>
+      <c r="G278" s="23"/>
       <c r="N278" s="14"/>
     </row>
     <row r="279" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E279" s="14"/>
+      <c r="G279" s="23"/>
       <c r="N279" s="14"/>
     </row>
     <row r="280" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E280" s="14"/>
+      <c r="G280" s="23"/>
       <c r="N280" s="14"/>
     </row>
     <row r="281" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E281" s="14"/>
+      <c r="G281" s="23"/>
       <c r="N281" s="14"/>
     </row>
     <row r="282" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E282" s="14"/>
+      <c r="G282" s="23"/>
       <c r="N282" s="14"/>
     </row>
     <row r="283" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E283" s="14"/>
+      <c r="G283" s="23"/>
       <c r="N283" s="14"/>
     </row>
     <row r="284" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E284" s="14"/>
+      <c r="G284" s="23"/>
       <c r="N284" s="14"/>
     </row>
     <row r="285" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E285" s="14"/>
+      <c r="G285" s="23"/>
       <c r="N285" s="14"/>
     </row>
     <row r="286" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E286" s="14"/>
+      <c r="G286" s="23"/>
       <c r="N286" s="14"/>
     </row>
     <row r="287" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E287" s="14"/>
+      <c r="G287" s="23"/>
       <c r="N287" s="14"/>
     </row>
     <row r="288" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E288" s="14"/>
+      <c r="G288" s="23"/>
       <c r="N288" s="14"/>
     </row>
     <row r="289" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E289" s="14"/>
+      <c r="G289" s="23"/>
       <c r="N289" s="14"/>
     </row>
     <row r="290" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E290" s="14"/>
+      <c r="G290" s="23"/>
       <c r="N290" s="14"/>
     </row>
     <row r="291" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E291" s="14"/>
+      <c r="G291" s="23"/>
       <c r="N291" s="14"/>
     </row>
     <row r="292" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E292" s="14"/>
+      <c r="G292" s="23"/>
       <c r="N292" s="14"/>
     </row>
     <row r="293" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E293" s="14"/>
+      <c r="G293" s="23"/>
       <c r="N293" s="14"/>
     </row>
     <row r="294" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E294" s="14"/>
+      <c r="G294" s="23"/>
       <c r="N294" s="14"/>
     </row>
     <row r="295" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E295" s="14"/>
+      <c r="G295" s="23"/>
       <c r="N295" s="14"/>
     </row>
     <row r="296" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E296" s="14"/>
+      <c r="G296" s="23"/>
       <c r="N296" s="14"/>
     </row>
     <row r="297" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E297" s="14"/>
+      <c r="G297" s="23"/>
       <c r="N297" s="14"/>
     </row>
     <row r="298" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E298" s="14"/>
+      <c r="G298" s="23"/>
       <c r="N298" s="14"/>
     </row>
     <row r="299" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E299" s="14"/>
+      <c r="G299" s="23"/>
       <c r="N299" s="14"/>
     </row>
     <row r="300" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E300" s="14"/>
+      <c r="G300" s="23"/>
       <c r="N300" s="14"/>
     </row>
     <row r="301" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E301" s="14"/>
+      <c r="G301" s="23"/>
       <c r="N301" s="14"/>
     </row>
     <row r="302" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E302" s="14"/>
+      <c r="G302" s="23"/>
       <c r="N302" s="14"/>
     </row>
     <row r="303" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E303" s="14"/>
+      <c r="G303" s="23"/>
       <c r="N303" s="14"/>
     </row>
     <row r="304" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E304" s="14"/>
+      <c r="G304" s="23"/>
       <c r="N304" s="14"/>
     </row>
     <row r="305" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E305" s="14"/>
+      <c r="G305" s="23"/>
       <c r="N305" s="14"/>
     </row>
     <row r="306" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E306" s="14"/>
+      <c r="G306" s="23"/>
       <c r="N306" s="14"/>
     </row>
     <row r="307" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E307" s="14"/>
+      <c r="G307" s="23"/>
       <c r="N307" s="14"/>
     </row>
     <row r="308" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E308" s="14"/>
+      <c r="G308" s="23"/>
       <c r="N308" s="14"/>
     </row>
     <row r="309" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E309" s="14"/>
+      <c r="G309" s="23"/>
       <c r="N309" s="14"/>
     </row>
     <row r="310" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E310" s="14"/>
+      <c r="G310" s="23"/>
       <c r="N310" s="14"/>
     </row>
     <row r="311" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E311" s="14"/>
+      <c r="G311" s="23"/>
       <c r="N311" s="14"/>
     </row>
     <row r="312" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E312" s="14"/>
+      <c r="G312" s="23"/>
       <c r="N312" s="14"/>
     </row>
     <row r="313" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E313" s="14"/>
+      <c r="G313" s="23"/>
       <c r="N313" s="14"/>
     </row>
     <row r="314" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E314" s="14"/>
+      <c r="G314" s="23"/>
       <c r="N314" s="14"/>
     </row>
     <row r="315" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E315" s="14"/>
+      <c r="G315" s="23"/>
       <c r="N315" s="14"/>
     </row>
     <row r="316" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E316" s="14"/>
+      <c r="G316" s="23"/>
       <c r="N316" s="14"/>
     </row>
     <row r="317" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E317" s="14"/>
+      <c r="G317" s="23"/>
       <c r="N317" s="14"/>
     </row>
     <row r="318" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E318" s="14"/>
+      <c r="G318" s="23"/>
       <c r="N318" s="14"/>
     </row>
     <row r="319" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E319" s="14"/>
+      <c r="G319" s="23"/>
       <c r="N319" s="14"/>
     </row>
     <row r="320" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E320" s="14"/>
+      <c r="G320" s="23"/>
       <c r="N320" s="14"/>
     </row>
-    <row r="321" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="321" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E321" s="14"/>
+      <c r="G321" s="23"/>
       <c r="N321" s="14"/>
     </row>
-    <row r="322" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="322" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E322" s="14"/>
+      <c r="G322" s="23"/>
       <c r="N322" s="14"/>
     </row>
-    <row r="323" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="323" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E323" s="14"/>
+      <c r="G323" s="23"/>
       <c r="N323" s="14"/>
     </row>
-    <row r="324" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="324" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E324" s="14"/>
+      <c r="G324" s="23"/>
       <c r="N324" s="14"/>
     </row>
-    <row r="325" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="325" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E325" s="14"/>
+      <c r="G325" s="23"/>
       <c r="N325" s="14"/>
     </row>
-    <row r="326" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="326" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E326" s="14"/>
+      <c r="G326" s="23"/>
       <c r="N326" s="14"/>
     </row>
-    <row r="327" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="327" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E327" s="14"/>
+      <c r="G327" s="23"/>
       <c r="N327" s="14"/>
     </row>
-    <row r="328" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="328" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E328" s="14"/>
+      <c r="G328" s="23"/>
       <c r="N328" s="14"/>
     </row>
-    <row r="329" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="329" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E329" s="14"/>
+      <c r="G329" s="23"/>
       <c r="N329" s="14"/>
     </row>
-    <row r="330" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="330" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E330" s="14"/>
+      <c r="G330" s="23"/>
       <c r="N330" s="14"/>
     </row>
-    <row r="331" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="331" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E331" s="14"/>
+      <c r="G331" s="23"/>
       <c r="N331" s="14"/>
     </row>
-    <row r="332" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="332" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E332" s="14"/>
+      <c r="G332" s="23"/>
       <c r="N332" s="14"/>
     </row>
-    <row r="333" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="333" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E333" s="14"/>
+      <c r="G333" s="23"/>
       <c r="N333" s="14"/>
     </row>
-    <row r="334" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="334" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E334" s="14"/>
+      <c r="G334" s="23"/>
       <c r="N334" s="14"/>
     </row>
-    <row r="335" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="335" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E335" s="14"/>
+      <c r="G335" s="23"/>
       <c r="N335" s="14"/>
     </row>
-    <row r="336" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="336" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E336" s="14"/>
+      <c r="G336" s="23"/>
       <c r="N336" s="14"/>
     </row>
-    <row r="337" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="337" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E337" s="14"/>
+      <c r="G337" s="23"/>
       <c r="N337" s="14"/>
     </row>
-    <row r="338" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="338" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E338" s="14"/>
+      <c r="G338" s="23"/>
       <c r="N338" s="14"/>
     </row>
-    <row r="339" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="339" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E339" s="14"/>
+      <c r="G339" s="23"/>
       <c r="N339" s="14"/>
     </row>
-    <row r="340" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="340" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E340" s="14"/>
+      <c r="G340" s="23"/>
       <c r="N340" s="14"/>
     </row>
-    <row r="341" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="341" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E341" s="14"/>
+      <c r="G341" s="23"/>
       <c r="N341" s="14"/>
     </row>
-    <row r="342" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="342" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E342" s="14"/>
+      <c r="G342" s="23"/>
       <c r="N342" s="14"/>
     </row>
-    <row r="343" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="343" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E343" s="14"/>
+      <c r="G343" s="23"/>
       <c r="N343" s="14"/>
     </row>
-    <row r="344" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="344" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E344" s="14"/>
+      <c r="G344" s="23"/>
       <c r="N344" s="14"/>
     </row>
-    <row r="345" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="345" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E345" s="14"/>
+      <c r="G345" s="23"/>
       <c r="N345" s="14"/>
     </row>
-    <row r="346" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="346" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E346" s="14"/>
+      <c r="G346" s="23"/>
       <c r="N346" s="14"/>
     </row>
-    <row r="347" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="347" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E347" s="14"/>
+      <c r="G347" s="23"/>
       <c r="N347" s="14"/>
     </row>
-    <row r="348" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="348" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E348" s="14"/>
+      <c r="G348" s="23"/>
       <c r="N348" s="14"/>
     </row>
-    <row r="349" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="349" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E349" s="14"/>
+      <c r="G349" s="23"/>
       <c r="N349" s="14"/>
     </row>
-    <row r="350" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="350" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E350" s="14"/>
+      <c r="G350" s="23"/>
       <c r="N350" s="14"/>
     </row>
-    <row r="351" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="351" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E351" s="14"/>
+      <c r="G351" s="23"/>
       <c r="N351" s="14"/>
     </row>
-    <row r="352" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="352" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E352" s="14"/>
+      <c r="G352" s="23"/>
       <c r="N352" s="14"/>
     </row>
-    <row r="353" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="353" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E353" s="14"/>
+      <c r="G353" s="23"/>
       <c r="N353" s="14"/>
     </row>
-    <row r="354" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="354" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E354" s="14"/>
+      <c r="G354" s="23"/>
       <c r="N354" s="14"/>
     </row>
-    <row r="355" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="355" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E355" s="14"/>
+      <c r="G355" s="23"/>
       <c r="N355" s="14"/>
     </row>
-    <row r="356" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="356" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E356" s="14"/>
+      <c r="G356" s="23"/>
       <c r="N356" s="14"/>
     </row>
-    <row r="357" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="357" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E357" s="14"/>
+      <c r="G357" s="23"/>
       <c r="N357" s="14"/>
     </row>
-    <row r="358" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="358" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E358" s="14"/>
+      <c r="G358" s="23"/>
       <c r="N358" s="14"/>
     </row>
-    <row r="359" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="359" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E359" s="14"/>
+      <c r="G359" s="23"/>
       <c r="N359" s="14"/>
     </row>
-    <row r="360" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="360" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E360" s="14"/>
+      <c r="G360" s="23"/>
       <c r="N360" s="14"/>
     </row>
-    <row r="361" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="361" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E361" s="14"/>
+      <c r="G361" s="23"/>
       <c r="N361" s="14"/>
     </row>
-    <row r="362" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="362" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E362" s="14"/>
+      <c r="G362" s="23"/>
       <c r="N362" s="14"/>
     </row>
-    <row r="363" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="363" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E363" s="14"/>
+      <c r="G363" s="23"/>
       <c r="N363" s="14"/>
     </row>
-    <row r="364" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="364" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E364" s="14"/>
+      <c r="G364" s="23"/>
       <c r="N364" s="14"/>
     </row>
-    <row r="365" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="365" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E365" s="14"/>
+      <c r="G365" s="23"/>
       <c r="N365" s="14"/>
     </row>
-    <row r="366" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="366" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E366" s="14"/>
+      <c r="G366" s="23"/>
       <c r="N366" s="14"/>
     </row>
-    <row r="367" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="367" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E367" s="14"/>
+      <c r="G367" s="23"/>
       <c r="N367" s="14"/>
     </row>
-    <row r="368" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="368" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E368" s="14"/>
+      <c r="G368" s="23"/>
       <c r="N368" s="14"/>
     </row>
-    <row r="369" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="369" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E369" s="14"/>
+      <c r="G369" s="23"/>
       <c r="N369" s="14"/>
     </row>
-    <row r="370" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="370" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E370" s="14"/>
+      <c r="G370" s="23"/>
       <c r="N370" s="14"/>
     </row>
-    <row r="371" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="371" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E371" s="14"/>
+      <c r="G371" s="23"/>
       <c r="N371" s="14"/>
     </row>
-    <row r="372" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="372" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E372" s="14"/>
+      <c r="G372" s="23"/>
       <c r="N372" s="14"/>
     </row>
-    <row r="373" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="373" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E373" s="14"/>
+      <c r="G373" s="23"/>
       <c r="N373" s="14"/>
     </row>
-    <row r="374" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="374" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E374" s="14"/>
+      <c r="G374" s="23"/>
       <c r="N374" s="14"/>
     </row>
-    <row r="375" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="375" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E375" s="14"/>
+      <c r="G375" s="23"/>
       <c r="N375" s="14"/>
     </row>
-    <row r="376" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="376" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E376" s="14"/>
+      <c r="G376" s="23"/>
       <c r="N376" s="14"/>
+    </row>
+    <row r="377" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E377" s="14"/>
+      <c r="G377" s="23"/>
+    </row>
+    <row r="378" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E378" s="14"/>
+      <c r="G378" s="23"/>
+    </row>
+    <row r="379" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E379" s="14"/>
+      <c r="G379" s="23"/>
+    </row>
+    <row r="380" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E380" s="14"/>
+      <c r="G380" s="23"/>
+    </row>
+    <row r="381" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E381" s="14"/>
+      <c r="G381" s="23"/>
+    </row>
+    <row r="382" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E382" s="14"/>
+      <c r="G382" s="23"/>
+    </row>
+    <row r="383" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E383" s="14"/>
+      <c r="G383" s="23"/>
+    </row>
+    <row r="384" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E384" s="14"/>
+      <c r="G384" s="23"/>
+    </row>
+    <row r="385" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E385" s="14"/>
+      <c r="G385" s="23"/>
+    </row>
+    <row r="386" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E386" s="14"/>
+      <c r="G386" s="23"/>
+    </row>
+    <row r="387" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E387" s="14"/>
+      <c r="G387" s="23"/>
+    </row>
+    <row r="388" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E388" s="14"/>
+      <c r="G388" s="23"/>
+    </row>
+    <row r="389" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E389" s="14"/>
+      <c r="G389" s="23"/>
+    </row>
+    <row r="390" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E390" s="14"/>
+      <c r="G390" s="23"/>
+    </row>
+    <row r="391" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E391" s="14"/>
+      <c r="G391" s="23"/>
+    </row>
+    <row r="392" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E392" s="14"/>
+      <c r="G392" s="23"/>
+    </row>
+    <row r="393" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E393" s="14"/>
+      <c r="G393" s="23"/>
+    </row>
+    <row r="394" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E394" s="14"/>
+      <c r="G394" s="23"/>
+    </row>
+    <row r="395" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E395" s="14"/>
+      <c r="G395" s="23"/>
+    </row>
+    <row r="396" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E396" s="14"/>
+      <c r="G396" s="23"/>
+    </row>
+    <row r="397" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E397" s="14"/>
+      <c r="G397" s="23"/>
+    </row>
+    <row r="398" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E398" s="14"/>
+      <c r="G398" s="23"/>
+    </row>
+    <row r="399" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E399" s="14"/>
+      <c r="G399" s="23"/>
+    </row>
+    <row r="400" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E400" s="14"/>
+      <c r="G400" s="23"/>
+    </row>
+    <row r="401" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E401" s="14"/>
+      <c r="G401" s="23"/>
+    </row>
+    <row r="402" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E402" s="14"/>
+      <c r="G402" s="23"/>
+    </row>
+    <row r="403" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E403" s="14"/>
+      <c r="G403" s="23"/>
+    </row>
+    <row r="404" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E404" s="14"/>
+      <c r="G404" s="23"/>
+    </row>
+    <row r="405" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E405" s="14"/>
+      <c r="G405" s="23"/>
+    </row>
+    <row r="406" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E406" s="14"/>
+      <c r="G406" s="23"/>
+    </row>
+    <row r="407" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E407" s="14"/>
+      <c r="G407" s="23"/>
+    </row>
+    <row r="408" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E408" s="14"/>
+      <c r="G408" s="23"/>
+    </row>
+    <row r="409" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E409" s="14"/>
+      <c r="G409" s="23"/>
+    </row>
+    <row r="410" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E410" s="14"/>
+      <c r="G410" s="23"/>
+    </row>
+    <row r="411" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E411" s="14"/>
+      <c r="G411" s="23"/>
+    </row>
+    <row r="412" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E412" s="14"/>
+      <c r="G412" s="23"/>
+    </row>
+    <row r="413" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E413" s="14"/>
+      <c r="G413" s="23"/>
+    </row>
+    <row r="414" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E414" s="14"/>
+      <c r="G414" s="23"/>
+    </row>
+    <row r="415" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E415" s="14"/>
+      <c r="G415" s="23"/>
+    </row>
+    <row r="416" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E416" s="14"/>
+      <c r="G416" s="23"/>
+    </row>
+    <row r="417" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E417" s="14"/>
+      <c r="G417" s="23"/>
+    </row>
+    <row r="418" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E418" s="14"/>
+      <c r="G418" s="23"/>
+    </row>
+    <row r="419" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E419" s="14"/>
+      <c r="G419" s="23"/>
+    </row>
+    <row r="420" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E420" s="14"/>
+      <c r="G420" s="23"/>
+    </row>
+    <row r="421" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E421" s="14"/>
+      <c r="G421" s="23"/>
+    </row>
+    <row r="422" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E422" s="14"/>
+      <c r="G422" s="23"/>
+    </row>
+    <row r="423" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E423" s="14"/>
+      <c r="G423" s="23"/>
+    </row>
+    <row r="424" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E424" s="14"/>
+      <c r="G424" s="23"/>
+    </row>
+    <row r="425" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E425" s="14"/>
+      <c r="G425" s="23"/>
+    </row>
+    <row r="426" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E426" s="14"/>
+      <c r="G426" s="23"/>
+    </row>
+    <row r="427" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E427" s="14"/>
+      <c r="G427" s="23"/>
+    </row>
+    <row r="428" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E428" s="14"/>
+      <c r="G428" s="23"/>
+    </row>
+    <row r="429" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E429" s="14"/>
+      <c r="G429" s="23"/>
+    </row>
+    <row r="430" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E430" s="14"/>
+      <c r="G430" s="23"/>
+    </row>
+    <row r="431" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E431" s="14"/>
+      <c r="G431" s="23"/>
+    </row>
+    <row r="432" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E432" s="14"/>
+      <c r="G432" s="23"/>
+    </row>
+    <row r="433" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E433" s="14"/>
+      <c r="G433" s="23"/>
+    </row>
+    <row r="434" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E434" s="14"/>
+      <c r="G434" s="23"/>
+    </row>
+    <row r="435" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E435" s="14"/>
+      <c r="G435" s="23"/>
+    </row>
+    <row r="436" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E436" s="14"/>
+      <c r="G436" s="23"/>
+    </row>
+    <row r="437" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E437" s="14"/>
+      <c r="G437" s="23"/>
+    </row>
+    <row r="438" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E438" s="14"/>
+      <c r="G438" s="23"/>
+    </row>
+    <row r="439" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E439" s="14"/>
+      <c r="G439" s="23"/>
+    </row>
+    <row r="440" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E440" s="14"/>
+      <c r="G440" s="23"/>
+    </row>
+    <row r="441" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E441" s="14"/>
+      <c r="G441" s="23"/>
+    </row>
+    <row r="442" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E442" s="14"/>
+      <c r="G442" s="23"/>
+    </row>
+    <row r="443" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E443" s="14"/>
+      <c r="G443" s="23"/>
+    </row>
+    <row r="444" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E444" s="14"/>
+      <c r="G444" s="23"/>
+    </row>
+    <row r="445" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E445" s="14"/>
+      <c r="G445" s="23"/>
+    </row>
+    <row r="446" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E446" s="14"/>
+      <c r="G446" s="23"/>
+    </row>
+    <row r="447" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E447" s="14"/>
+      <c r="G447" s="23"/>
+    </row>
+    <row r="448" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E448" s="14"/>
+      <c r="G448" s="23"/>
+    </row>
+    <row r="449" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E449" s="14"/>
+      <c r="G449" s="23"/>
+    </row>
+    <row r="450" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E450" s="14"/>
+      <c r="G450" s="23"/>
+    </row>
+    <row r="451" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E451" s="14"/>
+      <c r="G451" s="23"/>
+    </row>
+    <row r="452" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E452" s="14"/>
+      <c r="G452" s="23"/>
+    </row>
+    <row r="453" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E453" s="14"/>
+      <c r="G453" s="23"/>
+    </row>
+    <row r="454" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E454" s="14"/>
+      <c r="G454" s="23"/>
+    </row>
+    <row r="455" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E455" s="14"/>
+      <c r="G455" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
enny06 2019/10/04 19.15 Update print master item
</commit_message>
<xml_diff>
--- a/assets/templates/template_items_log.xlsx
+++ b/assets/templates/template_items_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\greebel\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0472CFA-DF9A-48A3-B3DB-C78138196697}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5A183B-CB25-46B2-8649-13D8688CB312}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="9705" xr2:uid="{2D745729-4032-447E-85FB-C820FC51974E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2D745729-4032-447E-85FB-C820FC51974E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -503,7 +503,7 @@
   <dimension ref="A1:O533"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,9 +601,9 @@
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>

</xml_diff>

<commit_message>
enny06 2019/10/07 16.47 Update print excel master item
</commit_message>
<xml_diff>
--- a/assets/templates/template_items_log.xlsx
+++ b/assets/templates/template_items_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\greebel\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5A183B-CB25-46B2-8649-13D8688CB312}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAD1126-6262-40FA-97D9-088986A17D3D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2D745729-4032-447E-85FB-C820FC51974E}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="18165" windowHeight="9705" xr2:uid="{2D745729-4032-447E-85FB-C820FC51974E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -117,20 +117,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -185,7 +176,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D347ED-B861-48B8-96B5-A98AF875B3CE}">
   <dimension ref="A1:O533"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,8 +591,8 @@
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="5"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>

</xml_diff>

<commit_message>
enny06 2019/10/08 14.29 Update print excel master items
</commit_message>
<xml_diff>
--- a/assets/templates/template_items_log.xlsx
+++ b/assets/templates/template_items_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\greebel\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAD1126-6262-40FA-97D9-088986A17D3D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC70A465-C35A-4D9B-9EFD-7B46152BDF1C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="18165" windowHeight="9705" xr2:uid="{2D745729-4032-447E-85FB-C820FC51974E}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="18165" windowHeight="9705" xr2:uid="{2D745729-4032-447E-85FB-C820FC51974E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,13 +35,13 @@
     <t>Item Code  :</t>
   </si>
   <si>
-    <t>Vendor     :</t>
+    <t>Awal  s/d  Akhir</t>
   </si>
   <si>
-    <t>Group   :</t>
+    <t>Vendor      :</t>
   </si>
   <si>
-    <t>Awal  s/d  Akhir</t>
+    <t>Group        :</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
   <dimension ref="A1:O533"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +524,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="9"/>
@@ -541,7 +541,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
@@ -557,7 +557,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>

</xml_diff>